<commit_message>
update app and data
</commit_message>
<xml_diff>
--- a/excel_files/bon_appetit_recipes.xlsx
+++ b/excel_files/bon_appetit_recipes.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:F90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -374,15 +374,20 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Summary</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Ingredients</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Instructions</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Image</t>
         </is>
@@ -401,15 +406,20 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>Inspired by salty-crunchy Sichuan dry-fried string beans (gan bian si ji dou), these green beans are shriveled and browned into delicious submission before receiving a flavor bomb of garlic, red pepper flakes, and chopped capers at the very end. Resist the urge to stir the beans around in the pan, and let them take on color like you would ground meat. Patience is essential here.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>['⅓ cup extra-virgin olive oil', '1 lb. green beans, trimmed, patted dry of any surface moisture or condensation', 'Kosher salt', '6 garlic cloves, sliced', '1 Tbsp. capers, drained, chopped', '1 tsp. crushed red pepper flakes']</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>['Heat oil in a large skillet over high until shimmering. Add green beans (the dryer they are, the less they will spatter when they hit the oil) and cook, covering skillet as needed if beans are spattering, until browned underneath, about 3 minutes. Turn beans with tongs and redistribute so they brown evenly (don’t toss them since hot oil can easily slosh out of skillet if you try to show off). Continue to cook, turning occasionally, until browned all over and tender, about 5 minutes longer. Season with salt. Add garlic, capers, and red pepper flakes. Cook, tossing occasionally, just until garlic turns golden, about 1 minute.', 'Transfer beans to a platter. Spoon caper-garlic mixture over and pour some oil over too; season with salt.']</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/5c38c88f3a94835decfc5934/16:9/w_940,c_limit/crispy-fried-green-beans.jpg</t>
         </is>
@@ -428,15 +438,20 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>We transformed the regular hands-on skillet method to a very hands-off oven technique.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>['4 pounds russet potatoes, peeled', '1 tablespoon kosher salt, plus more', '2 tablespoons olive oil, plus more', '2 onions, thinly sliced', '1 tablespoon distilled white vinegar', 'Freshly ground black pepper', 'Flaky sea salt']</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>['Parboil potatoes in a large pot of boiling salted water just until a paring knife slides into the center with some resistance, 15–20 minutes. Drain; transfer to a rimmed baking sheet and chill uncovered until cold, at least 30 minutes.', 'Place racks in highest and lowest positions in oven; preheat to 425°. Line two 8" cake pans with parchment; brush with 2 Tbsp. oil. Toss onions, vinegar, and 1 Tbsp. kosher salt in a large bowl. Let sit until onions are softened, 5–10 minutes (massage gently to speed up process).', 'Meanwhile, grate parboiled potatoes on a box grater or in a food processor, or cut using a julienne slicer. Place prepared pans on lower rack and heat 5 minutes.', 'Add potatoes to onion mixture and toss to combine; season with kosher salt and pepper. Divide potato mixture between hot pans and press down as firmly as possible to compact (a thin flexible spatula works well). Place on lower rack and bake until potatoes are very brown around the edges, 45–60 minutes. Remove rösti from oven; let cool slightly.', 'Heat broiler. Broil rösti on upper rack until tops are golden brown all over. Cut around sides with a small knife or offset spatula to loosen and invert rösti onto a wire rack set inside a rimmed baking sheet. Carefully remove parchment paper (if potatoes stick, let cool slightly). Brush top of rösti with more oil, sprinkle with sea salt, and broil until second side is deep golden brown.', 'Do Ahead: Potatoes can be parboiled 1 day ahead; once cold, cover. Rösti can be made 3 hours ahead; store uncovered at room temperature (or keep warm in a 250° oven up to 1 hour). Reheat in a 300° oven for 10 minutes before serving.']</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/57acd70af1c801a1038bc7ff/16:9/w_940,c_limit/salt-and-vinegar-rosti.jpg</t>
         </is>
@@ -455,15 +470,20 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>Risotto is like a clingy baby. You can’t put it down, you can’t walk away from it, and you can’t ignore it. Its needs are simple, it just wants all of you. And if you give it all of your patient attention, it will turn into a puddle of love. This simple, pure, unadulterated version stands up on its own, but it also makes an excellent canvas for seasonal ingredients—find out more about those toppings below. This is part of BA’s Best, a collection of our essential recipes.</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>['1 Tbsp. kosher salt, plus more', '6 Tbsp. extra-virgin olive oil', '½ large white onion, finely chopped (about 1½ cups)', '2 cups carnaroli or Japanese sushi rice', '1 cup dry white wine', '5 Tbsp. unsalted butter, cut into pieces', '1¾ cups finely grated Parmesan, divided', 'Freshly ground black pepper']</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>['Combine 1 Tbsp. salt and 10 cups water in a medium stockpot. Bring to a very bare simmer over medium heat.', 'Meanwhile, heat oil in a 6-qt. Dutch oven over medium. Cook onion and a pinch of salt, stirring frequently, until onion is translucent and starting to soften, 6–8 minutes. Add ½ cup water and cook, stirring often, until water evaporates and onion is sizzling in oil and completely tender, about 5 minutes. (Adding the water allows the onion to cook gently and thoroughly without taking on any color.) Taste onion; if it’s still firm at all, add another splash of water and continue cooking until meltingly soft.', 'Add rice and stir well to coat with oil. Cook, stirring constantly, until grains of rice are translucent around the edges and they make a glassy clattering sound when they hit the sides and bottom of pot, about 5 minutes. Coating the grains with oil before adding any liquid helps the rice cook evenly so that the outside does not become mushy before the center is tender. Add wine and another pinch of salt. Bring to a simmer and cook, stirring occasionally, until wine is completely evaporated, about 2 minutes.', 'Reduce heat to medium, then add hot salted water to rice in ¾-cup increments, stirring constantly and allowing liquid to absorb fully before adding more, until rice is al dente and surrounded by fluid, not-too-thick creamy suspension, 25–30 minutes. It should take 2–3 minutes for each addition to be absorbed; if things are moving faster than this, reduce heat to medium-low. Gradual absorption and constant agitation are key to encouraging the starches to release from the risotto, creating its trademark creamy consistency. You may not need all of the hot water, but err on the side of soup rather than sludge. The finished texture should be more of a liquid than a solid. Start checking the rice after about 15 minutes; the grains should be tender but not mushy, with a slightly firm center that doesn’t leave a chalky or bitty residue between your teeth after tasting. Do not overcook!', 'Remove pot from heat, add butter, and stir until melted. Gradually add 1¼ cups Parmesan, stirring until cheese is melted and liquid surrounding risotto is creamy but very fluid. Stir in more hot salted water if needed to achieve the right consistency. Taste and season with salt.', 'Divide risotto among warm bowls. Top each with a grind of pepper. Serve with remaining ½ cup Parmesan alongside for passing.', 'BA’s Best Risotto Parmigiano is good enough to serve on its own, but it’s also an excellent canvas for a whole host of toppings. Here are a few options we love, for whatever season you’re in.Photo by TED + CHELSEA CAVANAUGH, Food Styling by Simon Andrews', 'Spring: Buttered Sugar Snap Peas with MintHeat 4 Tbsp. unsalted butter in a large skillet over medium until foaming, about 1 minute. Add finely chopped white and light green parts of 5 scallions, season with kosher salt and freshly ground black pepper, and cook, stirring occasionally, until scallions are bright green and aromatic, 1–2 minutes. Add 1 lb. sugar snap peas (trimmed, cut in half lengthwise), season again, and cook, tossing occasionally, until crisp-tender, 2–3 minutes. Remove from heat and stir in ½ cup sliced mint leaves. Spoon peas and any pan juices onto BA’s Best Risotto.Photo by TED + CHELSEA CAVANAUGH, Food Styling by Simon Andrews', 'Summer: Burst Cherry Tomato SauceHeat 2 Tbsp. unsalted butter and 2 Tbsp. extra-virgin olive oil in a large skillet over medium until butter is foaming. Add 4 crushed garlic cloves, season with kosher salt and freshly ground black pepper, and cook, stirring occasionally, until garlic is aromatic and starting to brown, 1–2 minutes. Add 2 pints cherry tomatoes and increase heat to medium-high. Cook, tossing frequently and pressing down on tomatoes with a wooden spoon to encourage skins to split, about 5 minutes. Add ½ tsp. red pepper flakes and toss to combine. Taste and season with kosher salt and freshly ground black pepper, if needed. Spoon tomatoes and pan sauce onto BA’s Best Risotto. Drizzle with oil.Photo by TED + CHELSEA CAVANAUGH, Food Styling by Simon Andrews', 'Fall: Browned Mushrooms with ThymeHeat ¼ cup extra-virgin olive oil in a large skillet over medium-high until shimmering. Add 1 lb. mushrooms (such as shiitake, crimini, or maitake, trimmed, caps torn into 2" pieces) and cook, tossing occasionally, until they begin to soften and release some liquid, 3–4 minutes. Season with kosher salt and freshly ground black pepper and cook, tossing occasionally, until deeply browned and tender, 8–10 minutes. Add 5 crushed garlic cloves, 2 Tbsp. unsalted butter, and 4–5 sprigs thyme and cook, tossing occasionally, until garlic softens and butter is golden brown, about 3 minutes more. Remove from heat and add 2 Tbsp. white wine vinegar or fresh lemon juice. Toss to coat, scraping up any browned bits from surface of pan. Pluck out thyme sprigs. Spoon mushroom mixture onto BA’s Best Risotto.Photo by TED + CHELSEA CAVANAUGH, Food Styling by Simon Andrews', 'Winter: Lemon and ChivesStir finely grated zest of 2 lemons, ½ cup thinly sliced chives, and 5 Tbsp. extra-virgin olive oil in a small bowl; season with kosher salt and freshly ground black pepper. As soon as BA’s Best Risotto is done, stir in 3 Tbsp. fresh lemon juice. Spoon lemon-chive mixture onto risotto.']</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/5c803ed5eda4a341526b6077/16:9/w_940,c_limit/risotto-5.jpg</t>
         </is>
@@ -482,15 +502,20 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>The sweet and salty flavor of the soy paste really shines here, so use the best-quality one you can find. We like Yu Ding Xing’s glutinous rice soy paste. This recipe is from Taiwanese-American cook Lisa Cheng Smith’s spectacular Lunar New Year feast. Find the rest of her menu here.</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>['1 lb. Chinese broccoli or broccolini, trimmed, cut in thirds crosswise', '¼ cup soy paste (such as Yu Ding Xing)']</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>['Set a steamer basket in a large pot filled with 1" water, cover pot, and bring water to a boil. Add broccoli to steamer basket, cover pot, and steam broccoli until crisp-tender, about 5 minutes.', 'Meanwhile, whisk soy paste and 2 Tbsp. water in a large bowl.', 'Arrange broccoli on a platter and drizzle sauce over.']</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/5dcc4914d4ee5800088bfad5/16:9/w_940,c_limit/Lunar-New-Year-Chinese-Broccoli.jpg</t>
         </is>
@@ -509,15 +534,20 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>A simple stovetop technique transforms turnips by deploying a secret ingredient that may be hiding in the back of your fridge.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>['1 pound small turnips, trimmed, scrubbed, cut into 1” wedges', '2 tablespoons white miso', '2 tablespoons unsalted butter', '1 teaspoon sugar', 'Kosher salt and freshly ground black pepper', '2 tablespoons fresh lemon juice']</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>['Combine turnips, miso, butter, and sugar in a medium skillet, then add water just to cover vegetables. Season with salt and pepper.', 'Bring to a boil over medium-high heat and cook turnips, turning occasionally, until they are tender and liquid is evaporated, 15–20 minutes.', 'Once all the liquid has cooked off, keep cooking turnips, tossing occasionally, until they are golden brown and caramelized and the sauce thickens and glazes the vegetables, about 5 minutes longer.', 'Add lemon juice and a splash of water to pan and swirl to coat turnips. Season with salt and pepper.']</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/57acf8a3f1c801a1038bc97d/16:9/w_940,c_limit/miso-glazed-turnips.jpg</t>
         </is>
@@ -536,15 +566,20 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>The key for this classic pesto recipe is to add the basil at the very end instead of blending everything all at once. That way the basil doesn’t get bruised or lose its flavor and maintains its vibrant green color. This is part of BA's Best, a collection of our essential recipes.</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>['½ cup pine nuts', '3 oz. Parmesan, grated (about ¾ cup)', '2 garlic cloves, finely grated', '6 cups basil leaves (about 3 bunches)', '¾ cup extra-virgin olive oil', '1 tsp. kosher salt']</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>['Preheat oven to 350°. Toast pine nuts on a rimmed baking sheet, tossing once halfway through, until golden brown, 5–7 minutes. Transfer to a food processor and let cool. Add cheese and garlic and pulse until finely ground, about 1 minute. Add basil and place the top back on. With the motor running, add oil in a slow and steady stream until pesto is mostly smooth, with just a few flecks of green, about 1 minute. Season with salt.', 'Do Ahead: Pesto can be made 1 day ahead. Top with ½" oil to prevent browning. Cover with plastic wrap, pressing directly onto surface, and chill.', 'Cooks’ Note: If you want to use this with pasta, cook 12 oz. dried pasta (we prefer long pasta for pesto) in a large pot of boiling salted water, stirring occasionally, until al dente. Drain, reserving ½ cup pasta cooking liquid.', 'Place pesto and 2 Tbsp. unsalted butter, cut into pieces, in a large bowl. Add pasta and ¼ cup pasta cooking liquid. Using tongs, toss vigorously, adding more pasta cooking liquid if needed, until pasta is glossy and well coated with sauce. Season with salt.', 'Divide pasta among bowls. Top with finely grated Parmesan.Photo by Alex Lau']</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/5b72f35c7278c24ab618f773/16:9/w_940,c_limit/ba-best-pesto-1.jpg</t>
         </is>
@@ -563,15 +598,20 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>This recipe is from Evan Funke, chef-owner of L.A.’s pasta temple, Felix Trattoria. Think of this as carbonara minus the eggs but still with massive amounts of flavor from guanciale, black pepper, and Pecorino. The secret to Funke’s supremely creamy (yet creamless!) sauce? Vigorously stirring the pasta with a wooden spoon as soon as it hits the sauce. This coaxes out the starch and helps the noodles bind with whatever fat you’re using to create, as he says, a truly “groovy” dish. The method transforms this simple guanciale fat and hot water emulsion into glossy perfection.</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>['1 Tbsp. black peppercorns', '8 oz. guanciale (salt-cured pork jowl)', '1¾ cups fresh fava beans (from about \t1¾ lb. pods) or frozen fava beans', '1 lb. bucatini', '2 oz. Pecorino Romano, finely grated (about 1 cup), plus more for serving']</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>['Place peppercorns in a bag, close, and coarsely crush with a rolling pin or heavy skillet (alternatively, you can crush them directly on a cutting board set inside a large rimmed baking sheet). Slice guanciale into ¼"-thick slabs, then slice slabs crosswise into ¼"-thick matchsticks.', 'If using fresh fava beans, cook in a large pot of boiling salted water until just tender (the best way to gauge doneness is to check one; be sure to slip it from its skin before tasting!), about 3 minutes. Using a spider or slotted spoon, transfer to a bowl of ice water; let cool. Drain and peel away outer skin from each bean; discard skins. Reserve pot with boiling water for cooking pasta.', 'Place guanciale in a dry large Dutch oven or other heavy pot and set over medium-high heat. Cook, stirring often with a wooden spoon, until golden brown and crisp, about 5 minutes. Add crushed peppercorns and stir once to combine. Add 1 cup hot tap water (using pasta cooking liquid here could make the dish too salty) and bring to a boil. Remove pot from heat and stir mixture aggressively to emulsify. Let sit until pasta is done.', 'Return reserved pot of water to a boil and cook pasta, stirring occasionally (if using frozen fava beans, add about 2 minutes before pasta is done), until al dente. Drain pasta and fava beans.']</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/5e6bb3ba9b123d000836fd04/16:9/w_940,c_limit/0420-Pasta-Bucatini-with-Fava-Beans.jpg</t>
         </is>
@@ -590,15 +630,20 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>How to make steakhouse-quality steak at home. Step 1: Buy a great steak from a great butcher. Step 2: Salt it liberally. Step 3: Gradually build up a crusty sear. Step 4: Butter. Butter?! Yep—butter. Browned, nutty butter will deliver toasty flavor to every bite. It’s the secret to pretty much all the great steakhouse dinners you’ve ever had.</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
           <t>['1 1¾"-thick bone-in rib eye (about 1½ lb.)', 'Kosher salt, freshly ground pepper', '2 tsp. vegetable oil', '3 Tbsp. unsalted butter', '2 sprigs rosemary', '2 garlic cloves, crushed', 'Flaky sea salt']</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>['Season steak generously with kosher salt and pepper and let sit at room temperature 1 hour.', 'Heat a dry large skillet, preferably cast iron, over medium-high, then add oil. As soon as oil is smoking, cook steak, turning every 2 minutes or so, until a deep brown crust forms and the internal temperature is a few degrees below your favored doneness (120°–125° for medium-rare), 8–10 minutes.', 'Add butter, rosemary, and garlic to skillet, tilt pan toward you so that butter pools on one side, and use a large spoon to continually baste steak with butter. Continue until butter is no longer bubbling and it smells nutty and is beginning to brown, about 1 minute. Transfer meat to a cutting board and let rest 10 minutes. (For medium-rare, your steak should reach an internal temperature of 125°–130°.)', 'Cut meat from bone and slice against the grain 1" thick. Spoon some infused brown butter over steak and sprinkle with sea salt.Read More: The 29 New Essential Recipes from the Bon Appétit Test Kitchen']</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/5ab520846ed79626bc263210/16:9/w_940,c_limit/butter-basted-steak.jpg</t>
         </is>
@@ -617,15 +662,20 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t>Don’t be afraid to take the leeks to the point where they almost look burnt. A well-charred exterior means the interiors will be creamy, soft, silky, and delightfully sweet.</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
           <t>['4 medium leeks (about 2½ lb.), white and pale green parts only, tough outer layers removed (root ends left intact)', '2 Tbsp. sherry vinegar or red wine vinegar', '2 tsp. honey', '2 Tbsp. extra-virgin olive oil, plus more for drizzling']</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>['Prepare a grill for high heat. Rinse off any sand and dirt from leeks and pat dry. Arrange directly on grate (no need to oil) and grill, turning every few minutes with tongs, until outsides are completely blackened (leeks should start to soften and may begin to release some juices), 12–16 minutes.', 'Transfer leeks to a cutting board and let rest 10 minutes (the interiors will continue to steam and get even softer as they cool).', 'While the leeks are resting, whisk vinegar and honey in a small bowl until honey dissolves. Set dressing aside.', 'Cut leeks on a diagonal into 1½"–2" pieces. Transfer to a medium bowl and toss with 2 Tbsp. oil; season with salt.', 'Transfer leeks to a platter and spoon reserved dressing over. Drizzle with more oil and season with pepper.']</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/5e5e818d58c694000852fc48/16:9/w_940,c_limit/Alliums-Charred-Leeks-Honey-and-Vinegar.jpg</t>
         </is>
@@ -644,15 +694,20 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>You don’t need to add liquid to the pot before cooking—the collards will release plenty while they’re in there. You can reduce the braising liquid as much or as little as you want once they’re done. We like to serve the greens a little saucy, but you can simmer until the liquid is slightly reduced if that’s what you prefer.</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t>['3 Tbsp. grapeseed or extra-virgin olive oil', '1 medium white onion, finely chopped', '6 oz. slab bacon, cut into 1x¼" lardons', 'Kosher salt, freshly ground pepper', '3 bunches collard greens (about 1¾ lb.)', '1 fresh red chile (such as Fresno), cut into thin rounds, seeds removed if desired', 'Louisiana-style hot sauce (for serving)', 'An Instant Pot or pressure cooker']</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>['Heat oil in Instant Pot on Sauté setting (or heat over medium-high if using another pressure cooker). Add onion and bacon, season with salt and pepper, and cook, stirring occasionally, until onions are softened and just beginning to brown and bacon has rendered some of its fat, 5–6 minutes.', 'Meanwhile, cut collard leaves away from stems; discard stems. Cut leaves in half through the midline. Stack leaves and cut crosswise into 1"-thick strips. Add collards and chile to pot, season again with salt and pepper, and cook, tossing frequently, until collards are shiny and wilted, 3–4 minutes. Lock lid and cook on high pressure 12 minutes.', 'Release pressure manually, then open lid and taste collards; adjust seasoning as needed. If there’s a lot of liquid in the pot, simmer on Sauté setting until reduced enough to lightly coat greens.', 'Transfer collard greens to a platter. Season with hot sauce as desired.']</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/5dc9b32a4337af00092cf417/16:9/w_940,c_limit/1119-GoLive-Instant-Pot-Collards-lede.jpg</t>
         </is>
@@ -671,15 +726,20 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
+          <t>Cutting those slits in the fish is key. They help the fish cook more quickly and make it easier to tell when it's done.</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
           <t>['1 bunch cilantro', '8 ounces tomatillos, husks removed, rinsed, coarsely chopped', '¼ cup drained jarred pickled jalapeños, plus 1 tablespoon (or more) brine from jar', 'Kosher salt', '3 cups vegetable oil', '1 1½–2-pound whole fish (such as black sea bass or red snapper), cleaned', 'Warm tortillas (for serving)']</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>['Trim cilantro at the point where it becomes more stem-y than leafy; set leaves with tender stems aside for serving. Coarsely chop about ½ cup worth of stems and place in a blender along with tomatillos, pickled jalapeños, and pickling liquid. Purée until smooth; taste and season sauce with salt and more pickling liquid if desired.', 'Heat oil in a large cast-iron skillet over high. Transfer fish to a cutting board and pat dry thoroughly with paper towels. With a sharp knife, make slashes crosswise on a diagonal along the body of the fish every 2" on both sides, cutting all the way down to the bone. Season fish generously inside and out with salt.', 'When the oil is hot—it should be shimmering, and when you drop a small piece of tortilla into the oil it should begin sizzling immediately—grip the fish firmly by the tail and carefully lower, head first, into skillet, making sure to lay it down away from you. (If the tail sticks out of the pan a bit, it’s not a huge deal.) Fry until flesh on bottom side is cooked through and skin is deeply browned and crisp, about 4 minutes. While the fish is frying, use a metal spoon to baste the inside of the fish’s head with a bit of hot oil periodically. Use tongs and a fish spatula to carefully turn fish over. Fry until flesh on second side is cooked through and skin is deeply browned and crisp, about 4 minutes. Transfer to a wire rack and season both sides with more salt.', 'Pour tomatillo sauce onto a rimmed platter and gently place fish on top. Tuck reserved cilantro into the cavity between the fish’s head and body and around the fish. Serve with tortillas.']</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a428f7654ad34116652c1/16:9/w_940,c_limit/fried-whole-fish-with-tomatillo-sauce.jpg</t>
         </is>
@@ -698,15 +758,20 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
+          <t>Avocado gives this refreshing drink the creamy, sippable texture of a milkshake but without a drop of dairy.</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
           <t>['1 small ripe avocado, pit removed', '5 Tbsp. fresh lime juice', '3 Tbsp. sugar', 'Tiny pinch of kosher salt']</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>['Scoop avocado flesh into a blender and add lime juice, sugar, salt, ½ cup ice cubes, and 2 cups cold water. Purée until smooth; blend in another splash of water if mixture is too thick. Pour into glasses, filled with ice if desired.']</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/5c6584a833a51d5ba1caca71/16:9/w_940,c_limit/avocado-water.jpg</t>
         </is>
@@ -725,15 +790,20 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
+          <t>Like deviled eggs—but faster, easier, more delicious, and fancier-sounding. This recipe calls for peperoncini, but most pickle-y things (cornichons, olives, that jar of dilly beans you've had for years) will work just as well.</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
           <t>['4 large eggs, room temperature', '2 jarred peperoncini in brine', '4 sprigs parsley', '¼ cup mayonnaise', '½ tsp. smoked or hot paprika', 'Kosher salt']</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>['Bring a small saucepan of water to a boil.', 'Using a spider or slotted spoon, carefully lower 4 eggs into boiling water. Set timer for 8 minutes. Fill a large bowl with ice water.', 'While eggs are boiling, do the rest of your prep: Drain 2 peperoncini. Remove stems and finely chop. Transfer to a small bowl.', 'Pick off leaves from 4 parsley sprigs and finely chop (discard stems). Add to bowl with peperoncini.', 'Mix ¼ cup mayonnaise and ½ tsp. paprika in another small bowl.', 'When timer goes off, remove eggs from boiling water with spider or slotted spoon and transfer to ice bath. Let cool 5 minutes.', 'Peel eggs, slice in half lengthwise, then sprinkle yolks with salt. Transfer eggs to a plate.', 'Top each egg with paprika mayo and peperoncini salsa.']</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/5a8478c28e5ab504d767b0c8/3:2/w_940,c_limit/eggs-paprika-aioli-sq.jpg</t>
         </is>
@@ -752,15 +822,20 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
+          <t>This classic lemon sauce recipe has a lot of fat and a lot of acidity, so don’t be shy with adding salt and taste as you go. It will likely require more than you think to strike that perfect balance.</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
           <t>['1 lemon', '12 oz. spaghetti or other long pasta', 'Kosher salt', '¾ cup heavy cream', '6 Tbsp. unsalted butter', '3 oz. finely grated Parmesan (about ¾ cup)', 'Freshly ground black pepper']</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>['Using a vegetable peeler, remove two 2"-long strips of lemon zest. Thinly slice each strip lengthwise into thin strands; set aside for serving. Finely grate remaining zest into a large pot (like a Dutch oven). Cut lemon in half and squeeze out enough juice to yield 2 Tbsp. into a small bowl; set aside.', 'Cook pasta in another large pot of boiling heavily salted water, stirring occasionally, until very al dente (pasta will finish cooking in the sauce).', 'Meanwhile, add cream to pot with lemon zest and cook over medium heat, whisking often, until liquid is just beginning to simmer, about 2 minutes. Reduce heat to medium-low. Whisk in butter 1 Tbsp. at a time until melted and sauce is creamy and emulsified. Remove from heat.', 'Just before pasta is al dente, scoop out 1½ cups pasta cooking liquid. Add ¾ cup pasta cooking liquid to cream sauce and return to medium heat. Using tongs, transfer spaghetti to pot with sauce (it’s okay if a little water comes along with it). Cook, tossing often and adding Parmesan little by little, until cheese is melted and sauce is creamy, about 3 minutes. If sauce looks tight, add 1–2 Tbsp. pasta cooking liquid. (Cream sauces tighten up very quickly as they cool, so it’s better to lean on the saucier side of things.) Stir in reserved lemon juice; season with more salt, if needed.', 'Divide pasta among bowls. Season with pepper, then top with reserved lemon zest strips.Photo by Chelsie Craig, Food Styling by Kate Buckens']</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/5b9a901947aaaf7cd9ea90f2/16:9/w_940,c_limit/ba-recipe-pasta-al-limone.jpg</t>
         </is>
@@ -779,15 +854,20 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
+          <t>The hardest part of this recipe is tracking down Thai tea mix (or waiting for it to arrive in the mail)—but it’s worth it. Tantalizingly vanilla-y and deeply spiced, it dials back the sweetness of the ice cream. And you’ll go through any leftovers quickly: Brew, pour over ice, and stir in sweetened condensed milk.</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
           <t>['2½ cups heavy cream, divided', '½ cup Thai tea mix (such as Pantai)', '1 tsp. vanilla extract', '1⅓ cups sweetened condensed milk (from one 14-oz. can), divided', '½ tsp. kosher salt, divided', '½ cup roasted, salted peanuts, very finely chopped']</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>['Bring 1½ cups cream to a bare simmer in a small saucepan over medium-low heat. Add tea mix, stir to combine, then remove from heat and let steep 30 minutes. Strain through a fine-mesh sieve into a glass measuring cup, pressing to push out all of the liquid (you should have about 1 cup; it’s okay if there are flecks of tea leaves). Chill until cold (use an ice bath to speed up the process, if you wish).', 'Beat vanilla, ⅔ cup condensed milk, ¼ tsp. salt, and remaining 1 cup cream in the bowl of a stand mixer fitted with the whisk attachment on low speed until combined. Increase speed to medium-high and continue to beat until the whisk leaves trails and you have soft peaks and a beautiful, billowy mixture, 2–3 minutes (you can also do this with hand-held beaters and a large bowl). Transfer to a large bowl, then use a rubber spatula to gently fold in peanuts. (It’s okay to leave big streaks of nuts!)', 'Pour chilled Thai tea cream into mixer bowl (no need to wipe out). Add remaining ⅔ cup condensed milk and ¼ tsp. salt. Beat on low speed until combined. Increase speed to medium-high and continue to beat until mixture looks just like the first one, 4–5 minutes. Be careful not to overbeat, as it can quickly go from creamy to grainy.', 'Scoop mixture into bowl with vanilla base, then gently fold the two together in just a few strokes so that you have big ripples of each. If you fold too many times, you’ll lose the swirls (but don’t worry; the flavor won’t suffer!). Transfer to a 9x5" loaf pan; smooth top. Cover with plastic wrap and freeze at least 6 hours.', 'Let ice cream sit at room temperature 5–7 minutes, then use an ice cream scoop dipped in hot water to distribute scoops among bowls.', 'Do Ahead: Ice cream can be made 1 week ahead. Keep frozen.Photo by Chelsie Craig, food styling by Kat Boytsova']</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/5d1cd16d43a78a00091b164e/16:9/w_940,c_limit/Thai-Iced-Tea-IceCream-lede.jpg</t>
         </is>
@@ -806,15 +886,20 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
+          <t>This tart recipe is the adult version of a certain toaster snack you loved as a kid but with a lot less sugar. This recipe was reader-requested from Gan Shan Station in Asheville, NC.</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
           <t>['1 tablespoon granulated sugar', '1½ teaspoons kosher salt', '3¼ cups all-purpose flour, plus more for surface', '¾ cup (1½ sticks) unsalted butter, cut into pieces', '3 large eggs', '½ cup homemade or store-bought jam (any flavor)', 'Raw sugar (for sprinkling)']</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>['Pulse granulated sugar, salt, and 3¼ cups flour in a food processor just to combine. Add butter and pulse until largest pieces are pea-size. Whisk 2 eggs and 4 Tbsp. ice water in a small bowl to blend, then drizzle into flour mixture and pulse just until mixture begins to clump together.', 'Turn out dough onto a work surface and knead, adding more ice water by the tablespoonful if needed, until dough comes together into a cohesive mass. Pat into a 6x4" rectangle and wrap tightly in plastic; chill at least 1 hour.', 'Preheat oven to 350°. Roll out dough on a lightly floured surface to an 18x14" rectangle, about ¼" thick. Trim away jagged edges to make a 16x12" rectangle. Using a bench scraper or pastry wheel, cut dough into sixteen 4x3" rectangles.', 'Beat remaining egg in a small bowl with 1 Tbsp. water. Brush a ½" strip of egg wash around edges of half of the rectangles. Dollop 1 Tbsp. jam in the center of each egg-washed rectangle. Top with remaining rectangles and gently press down around edges; crimp with a fork to seal. Brush tops of tarts with egg wash and sprinkle with raw sugar. Cut three slashes on a diagonal across the top of each tart. Transfer to a parchment-lined baking sheet and bake until crust is golden brown, 20–25 minutes. Transfer to a wire rack and let cool at least 1 hour before serving.', 'Do Ahead: Dough can be made 1 day ahead. Keep chilled.']</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a3e222b659b48a371c32e/16:9/w_940,c_limit/jam-toaster-tarts.jpg</t>
         </is>
@@ -833,15 +918,20 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
+          <t>This recipe method concentrates the berries’ flavors, so the more delicious they are to begin with, the better they will be dried. Here’s your opportunity to use up berries that are slightly past their prime. At Craftsman and Wolves in San Francisco, CA, William Werner combines them with raw berries in tarts or adds them to arugula salads. They're chewy—a bit softer than a dried apricot—with a plump, juicy consistency.</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
           <t>['1 pound strawberries, hulled, halved, quartered if large', '2 tablespoons raw sugar or granulated sugar']</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>['Toss strawberries and sugar in a large bowl and let sit until berries start to release their juices, 25–30 minutes.', 'Preheat oven to 185° (or the lowest possible setting, which may be 200°). Spread out berries on a rimmed baking sheet lined with a nonstick baking mat and bake, rotating baking sheet about every 30 minutes, until berries are darkened in color and dried out around the edges but still slightly juicy in the center, 3–3½ hours. Let cool on baking sheet.', 'Do Ahead: Berries can be dried 1 week ahead. Cover and chill.']</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a40705df40d1371270624/16:9/w_940,c_limit/oven-dried-strawberries.jpg</t>
         </is>
@@ -860,15 +950,20 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
+          <t>No more excuses for store-bought salad dressing: This jar vinaigrette, made only from staple ingredients, takes almost no time to assemble and will keep for up to a month.</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
           <t>['1½ cups extra-virgin olive oil', '¾ cup any combination red wine vinegar, white wine vinegar, and/or apple cider vinegar', '1 Tbsp. Dijon mustard', '1 Tbsp. honey', 'Kosher salt']</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>['Combine oil, vinegars, mustard, and honey in a large resealable jar or airtight container; cover and shake vigorously until emulsified, about 30 seconds. Season with salt.', 'Do Ahead: Vinaigrette can be made 1 month ahead. Cover and chill.']</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/5cbf8dafa25252714e911c1e/16:9/w_940,c_limit/new-standard-vinagrette-b.jpg</t>
         </is>
@@ -887,15 +982,20 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
+          <t>A little meat-mallet action transforms this tough cut of beef into a quick-grilling all-star. We cribbed the pounding technique from Chris Fischer's amazing The Beetlebung Farm Cookbook.</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
           <t>['1½ pounds zucchini, cut into ¼-inch pieces (about 5 cups)', '½ cup red wine vinegar', '1 tablespoon coarsely chopped oregano, plus leaves for serving', '¼ cup olive oil, plus more for steak', 'Kosher salt, freshly ground pepper', '1 1½-pound piece flank steak']</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>['Toss zucchini, vinegar, chopped oregano, and ¼ cup oil in a medium bowl to combine; season zucchini salsa with salt and pepper. Set aside.', 'Prepare a grill for high heat. Meanwhile, flatten your steak. Cover a cutting board with a long piece of plastic wrap and set steak on top; fold plastic over steak to cover. Using the smooth side of a meat mallet, pound steak to about ½" thick. (Don’t hold back; you want it good and roughed up.) Pat steak dry with paper towels; season generously with salt and rub a bit of oil all over. Grill until browned, about 2 minutes per side for medium-rare. (You might not get that much color on this steak because it’s so thin, but you don’t want it to be overcooked.) Transfer steak to a cutting board and let rest 5–10 minutes. Cut in half lengthwise with the grain, then slice thinly against the grain.', 'Arrange steak on a platter and spoon half of reserved salsa along with some juices over steak. Top with oregano leaves. Serve remaining salsa alongside.', 'Do Ahead: Zucchini salsa can be made 1 day ahead. Cover and chill.']</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a45787654ad34116652c3/16:9/w_940,c_limit/pounded-flank-steak-with-zucchini-salsa.jpg</t>
         </is>
@@ -914,15 +1014,20 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>['1 3½–4-lb. whole chicken,  patted dry', '8 green garlic stalks, dark green tops removed, divided', '6 Tbsp. unsalted butter, room temperature', '¼ cup extra-virgin olive oil']</t>
+          <t>Roasting a whole chicken quickly at high heat is optimal for the crispiest skin but risks overcooking the meat. This method of going low and slow is much gentler on the meat, keeping it juicy yet shreddable underneath skin that crackles. The green garlic has a mild, fresh flavor (much less bite than regular garlic, but you can use that here too). As the chicken cooks, the green garlic dries out and turns into a crispy crumb topping.</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>['Season chicken all over inside and out with salt and pepper (make sure to get in and around every nook and cranny; about 4 tsp. Diamond Crystal or 2½ tsp. Morton kosher salt). Place on a wire rack set inside a rimmed baking sheet and let sit at room temperature while you make the garlic butter, or chill, uncovered, up to 1 day. If chilling, let sit at room temperature 1 hour before roasting.', 'Place a rack in middle of oven; preheat to 325°. Coarsely chop 4 green garlic stalks; transfer to a food processor. Pulse until very finely chopped. Add zest and butter and pulse until almost smooth. Cut remaining 4 green garlic stalks in half lengthwise; set aside.', 'Pat chicken dry again with paper towels (this will help the butter adhere and get the skin nicely browned). Smear garlic butter all over chicken. Gently lift the skin on the breast away from the flesh and rub some butter inside.', 'Toss reserved green garlic and oil in a large cast-iron skillet or 13x9" baking dish to coat; season with salt. Tie chicken legs together with kitchen twine and tuck wings underneath back. Place chicken, breast side up, on top of garlic in skillet.', 'Roast chicken, rotating pan halfway through for even browning, until skin is golden and an instant-read thermometer inserted into the thickest part of breast registers 155° (don’t worry; temperature will climb to 165° as the chicken rests), 80–90 minutes. Let chicken rest at least 20 minutes and up to 45 minutes.', 'Transfer chicken to a cutting board and carve as desired. Serve with roasted green garlic alongside.']</t>
+          <t>['1 3½–4-lb. whole chicken,  patted dry', 'Kosher salt, freshly ground pepper', '8 green garlic stalks, dark green tops removed, divided', '6 Tbsp. unsalted butter, room temperature', '1 Tbsp. finely grated lemon zest', '¼ cup extra-virgin olive oil']</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
+        <is>
+          <t>['Season chicken all over inside and out with salt and pepper (make sure to get in and around every nook and cranny; about 4 tsp. Diamond Crystal or 2½ tsp. Morton kosher salt). Place on a wire rack set inside a rimmed baking sheet and let sit at room temperature while you make the garlic butter, or chill, uncovered, up to 1 day. If chilling, let sit at room temperature 1 hour before roasting.', 'Place a rack in middle of oven; preheat to 325°. Coarsely chop 4 green garlic stalks; transfer to a food processor. Pulse until very finely chopped. Add butter and zest and pulse until almost smooth. Cut remaining 4 green garlic stalks in half lengthwise; set aside.', 'Pat chicken dry again with paper towels (this will help the butter adhere and get the skin nicely browned). Smear garlic butter all over chicken. Gently lift the skin on the breast away from the flesh and rub some butter inside.', 'Toss reserved green garlic and oil in a large cast-iron skillet or 13x9" baking dish to coat; season with salt. Tie chicken legs together with kitchen twine and tuck wings underneath back. Place chicken, breast side up, on top of garlic in skillet.', 'Roast chicken, rotating pan halfway through for even browning, until skin is golden and an instant-read thermometer inserted into the thickest part of breast registers 155° (don’t worry; temperature will climb to 165° as the chicken rests), 80–90 minutes. Let chicken rest at least 20 minutes and up to 45 minutes.', 'Transfer chicken to a cutting board and carve as desired. Serve with roasted green garlic alongside.']</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/5e5d76655a099a000880933a/16:9/w_940,c_limit/Alliums-Garlic-Rubbed-Buttery-Roast-Chicken.jpg</t>
         </is>
@@ -941,15 +1046,20 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
+          <t>Eat standing up, ideally over the sink.</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
           <t>['1 cup drained jarred giardiniera, finely chopped, plus some brine from the jar', '1 cup mayonnaise', '4 8-inch soft Italian sub rolls, split', '4 large meaty tomatoes, sliced ½ inch thick', 'Kosher salt', '1 head of iceberg lettuce, thinly shredded', 'Freshly ground black pepper', 'Olive oil (for drizzling)']</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>['Mix giardiniera into mayonnaise in a small bowl. Thickly spread some giardiniera mixture over the bottom half of each roll. Top each with tomato slices; season with salt. Layer on a thick tuft of shredded lettuce; season lettuce with salt, pepper, and a splash of reserved giardiniera brine (about 1 Tbsp. per sandwich). Drizzle with oil.']</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a47327102712b68401aa7/16:9/w_940,c_limit/veggie-italian-hoagie.jpg</t>
         </is>
@@ -968,15 +1078,20 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
+          <t>This versatile peak-of-summer condiment can be served on top of white rice, pasta, toast, steamed fish, steak, or roast chicken. This recipe is part of the Healthyish Farmers’ Market Challenge. Get all 10 recipes here.</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
           <t>['4 tablespoons unsalted butter', '1 1-inch piece ginger, peeled, cut into thin matchsticks', '4 scallions, white and pale green parts finely chopped, dark green parts thinly sliced', '1½ pounds tomatoes, cut into 1-inch pieces (about 4 cups)', '2 tablespoons plus 1½ teaspoons white or regular soy sauce', 'Kosher salt']</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>['Heat butter in a large skillet over medium. As soon as butter stops foaming, add ginger and scallion whites and cook, stirring, until fragrant, about 1 minutes. Add tomatoes and cook, turning gently with a large spoon, until tomatoes are juicy and just warmed through, about 2 minutes. Add soy sauce and toss to combine. Taste and season with salt, if needed. Top with scallion greens.Alex Lau']</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="F23" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/5b5f17f0a6316e2d69db40f2/16:9/w_940,c_limit/healthyish-fmc-tomatotoastwide.jpg</t>
         </is>
@@ -995,15 +1110,20 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
+          <t>Seasoned with Old Bay, a little garlic, and some charred lemons, these grilled shrimp channel classic East Coast fish shack vibes. We highly encourage you eat them with the shells on—the crunchy texture and smoky flavor they pick up from the grill are all part of the pleasure. But if you’d rather not, go ahead and peel ’em before serving. Also, they’re just as delicious chilled as they are hot off the grill, so enjoy them whichever way you like.</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
           <t>['½ cup plus 1 Tbsp. canola oil, plus more for grill', '1 lb. shell-on shrimp (16–20 per lb.)', '3 small garlic cloves, finely grated, divided', '1½ tsp. Old Bay seasoning, plus more for serving', '¾ tsp. kosher salt, divided, plus more', '1 large egg yolk', '2 lemons, divided']</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>['Prepare a grill for medium-high heat. Lightly oil grate. Using kitchen shears, snip down back of each shrimp shell along the vein, stopping at the tails. You may end up cutting a little but of the flesh, but the aim here is to make it easy to peel the shell later (if you choose!) without compromising the shrimp’s tenderness. The shells are a protective barrier, so keep them on when grilling.', 'Transfer shrimp to a medium bowl. Add 1 Tbsp. oil, two-thirds of garlic, 1½ tsp. Old Bay, and ¾ tsp. salt and toss to combine. Let sit 10–15 minutes while you prepare the aioli.', 'Whisk egg yolk and remaining garlic in a medium bowl. Finely grate 1 tsp. lemon zest into egg mixture. Whisking constantly, gradually stream in remaining ½ cup oil until thick and pale yellow. Stir in juice of one lemon half. Season well with salt—it should taste really vibrant.', 'Cut remaining lemon in half. Grill shrimp and 3 lemon halves (cut sides down) until shells are golden brown and charred in some spots and flesh is opaque and cut sides of lemons are deeply caramelized, 1–2 minutes.', 'Spread aioli on a platter. Arrange shrimp and charred lemons over. Season lightly with more Old Bay.']</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="F24" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/5d49c7029a7d740009bc1e62/16:9/w_940,c_limit/ba-0819-old-bay-shrimp.jpg</t>
         </is>
@@ -1022,15 +1142,20 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
+          <t>This zippy, herbaceous drinkable soup is like a trip to the farmers’ market in a glass. Coldness dulls flavor, which is why it's important to season generously while the mixture is warm.</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
           <t>['2 pounds English hothouse cucumbers (about 2 large), chopped', '2 garlic cloves, smashed', '2 cups coarsely chopped arugula', '2 cups coarsely chopped mixed tender herbs (such as basil, parsley, cilantro, and/or mint)', '3 tablespoons (or more) sherry vinegar or red wine vinegar', 'Kosher salt', '¾ cup (or more) olive oil']</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>['Purée cucumbers, garlic, and ½ cup water in a blender until smooth. Add arugula, herbs, vinegar, and a large pinch of salt and purée, stopping to scrape down the sides of the blender as needed, until very smooth. With the motor running, slowly stream in oil; blend until emulsified. (The mixture will turn pale green and look creamy, almost like a salad dressing; add more oil and/or water if needed.) Taste gazpacho and season with more salt and vinegar as desired—you want it to be borderline too salty and acidic at room temperature. Transfer gazpacho to an airtight container; cover and chill until very cold, 4–12 hours.', 'Taste gazpacho and adjust with a little more salt and/or vinegar as needed just before pouring into chilled glasses.']</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="F25" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a44492b659b48a371c330/16:9/w_940,c_limit/sippin-green-gazpacho.jpg</t>
         </is>
@@ -1049,15 +1174,20 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
+          <t>If they’re in season, look for fresh peas. And if not, there is no shame in using frozen—it’s one of the few frozen vegetables we can get behind. This recipe is from Evan Funke, chef-owner of L.A.’s pasta temple, Felix Trattoria.</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
           <t>['1 lb. tagliatelle', '1½ cups shelled fresh peas (from about 1½ lb. pods) or frozen peas', '½ cup (1 stick) unsalted butter', '6 oz. prosciutto, thinly sliced (about 12 slices)', '16 sage leaves', '2 oz. Parmesan, finely grated (about 1 cup), plus more for serving']</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="E26" t="inlineStr">
         <is>
           <t>['Cook pasta in a large pot of boiling salted water, stirring occasionally and adding peas about 2 minutes before pasta is done, until al dente. Drain pasta and peas, reserving 1½ cups pasta cooking liquid.', 'Meanwhile, heat butter in a large Dutch oven or other heavy pot over medium until frothy. Tear prosciutto slices into bite-size pieces and add to pot along with sage. Cook, stirring occasionally, until prosciutto is golden brown and beginning to crisp, about 4 minutes. Remove from heat and let sit until pasta is done.', 'Add pasta, peas, 2 oz. Parmesan, and 1 cup reserved pasta cooking liquid to pot with prosciutto and return to medium heat. Cook, tossing vigorously and adding more pasta cooking liquid if needed, until saucy and pasta is coated, about 30 seconds. Taste and season with more salt if needed.', 'Divide pasta among bowls and top with more Parmesan.']</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="F26" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/5e6f8d676c81770008a583dd/16:9/w_940,c_limit/0420-Pasta-Tagliatelle-Prosciutto-and-Peas-NEW.jpg</t>
         </is>
@@ -1076,15 +1206,20 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
+          <t>Cooking fish doesn't need to be intimidating. In fact, few things could be simpler—or more rewarding. For meaty steaks of swordfish, albacore, and halibut, all you need is a kiss of high heat from a grill or cast-iron pan and a simple vinaigrette. Zesting citrus directly onto your food means no wasted precious aromatic oils and zero chance of the zest drying out before you use it.</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
           <t>['¼ cup olive oil, plus more for grill and drizzling', '1 lemon', '4 5–6-ounce skinless, boneless halibut fillets', 'Kosher salt, freshly ground pepper', '2 pounds mixed heirloom tomatoes, sliced', '½ cup sliced drained hearts of palm', 'Torn basil leaves (for serving)']</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t>['Prepare a grill for medium heat; oil grates. Finely grate 1 tsp. lemon zest directly onto halibut and lightly drizzle with oil; season with salt and pepper. Grill halibut, turning once, until browned on both sides and just opaque in the center, about 5 minutes.', 'Meanwhile, combine tomatoes, hearts of palm, and ¼ cup oil in a medium bowl; squeeze in 2 Tbsp. juice from lemon and toss to combine. Season with salt and pepper.', 'Toss basil into tomato salad. Serve halibut with tomatoes and dressing spooned over.']</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
+      <c r="F27" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a567b6c75df51bc0b91f2/16:9/w_940,c_limit/grilled-halibut-with-tomatoes-and-hearts-of-palm.jpg</t>
         </is>
@@ -1103,15 +1238,20 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
+          <t>It's not about the number of steps or ingredients in a dish. If you shop smart, buying peak-season produce and quality protein, you don't have to do much at all (like with this easy salad recipe). Read more about fruit caprese salad ideas here.</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
           <t>['8 ounces buffalo mozzarella or fresh mozzarella', '8 ounces ripe fresh figs, cut into quarters', 'Torn basil leaves (for serving)', 'Coarsely ground black pepper', 'Flaky sea salt', 'Olive oil (for drizzling)']</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="E28" t="inlineStr">
         <is>
           <t>['Tear mozzarella into medium pieces and arrange on a platter. Tuck figs around cheese and scatter basil over top. Season with pepper and lots of salt. Drizzle generously with oil.']</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="F28" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a3ccf5df40d1371270622/16:9/w_940,c_limit/adam-rapoports-fig-caprese.jpg</t>
         </is>
@@ -1130,15 +1270,20 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
+          <t>Though it may seem like a counterintuitive practice, extra flipping is the secret to the golden-brown crust on these pork chops.</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
           <t>['1 tablespoon vegetable oil', '2 1½”-thick bone-in pork rib chops (8–10 ounces each)', 'Kosher salt and freshly ground black pepper', '8 sprigs sage', '2 garlic cloves, peeled, smashed', '1 tablespoon unsalted butter']</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t>['Heat oil in a large skillet over medium-high. Season pork chops all over (including the fat cap) with salt and pepper. Cook pork chops until bottom side is golden brown, about 1 minute. Turn and cook on other side about 1 minute before turning again. Repeat this process, turning about every minute, until chops are deep golden brown and an instant-read thermometer inserted into the thickest part registers 135°, 8–10 minutes (cooking time will depend on thickness of chops).', 'Remove pan from heat and add sage, garlic, and butter, smashing garlic into butter. Tilt skillet and spoon foaming butter and drippings over pork chops, making sure to baste the fat cap as well as the rib. Transfer pork chops to a cutting board and let rest at least 5 minutes (pork will come to 145° as it sits).', 'Cut away bone and slice pork about ¼” thick. Serve with any juices from the cutting board spooned over top.']</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
+      <c r="F29" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/57acf5bd1b334044149753ab/16:9/w_940,c_limit/your-new-favorite-pork-chops.jpg</t>
         </is>
@@ -1157,15 +1302,20 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
+          <t>This basil-infused puréed watermelon punch will go fast, trust us! For a spicier kick in this punch recipe, swap regular basil for the Thai variety.</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
           <t>['1 2-pound baby seedless watermelon', '¾ cup (or more) sugar', '2 cups basil leaves, plus sprigs for serving', '1 750-ml bottle tequila blanco', '1 cup fresh lemon juice', 'Lemon wheels (for serving)']</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="E30" t="inlineStr">
         <is>
           <t>['If using watermelon as a punch bowl, cut a ½"-thick slice off the bottom so it will sit upright, then cut a 2"-thick slice off the top. Using a large metal spoon, scoop out flesh, being careful not to pierce the rind. To serve from a pitcher (easier!), cut away rind and slice flesh into 2" pieces.', 'Purée watermelon flesh and sugar in a blender until smooth and sugar is dissolved. Add 2 cups basil and blend on low speed until leaves are broken up, about 10 seconds (don’t overprocess). Let sit 15 minutes, then strain into a pitcher. Whisk in tequila and lemon juice; taste and add more sugar, if desired. Chill until cold, at least 1 hour and up to 4 hours.', 'Pour punch into watermelon set in a bowl of ice, or serve in ice-filled rocks glasses. Garnish with basil sprigs and lemon wheels.']</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
+      <c r="F30" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a5a572b659b48a371c334/16:9/w_940,c_limit/heat-to-heat-punch.jpg</t>
         </is>
@@ -1184,15 +1334,20 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
+          <t>What raw cucumbers lack in cheer, pickled cucumbers make up for in zip, zing, and crunch. The brine can work with any crunchy veg, but we like them best with cucumbers. We guarantee they'll be the sleeper hit of your next party spread.</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
           <t>['2 lb. medium Persian cucumbers (about 12), cut lengthwise into spears', '¼ cup white wine vinegar or unseasoned rice vinegar', '1 tsp. sugar', '¾ tsp. crushed red pepper flakes', '2 tsp. kosher salt, plus more', '2 Tbsp. chopped dill', '2 Tbsp. fresh lemon juice']</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="E31" t="inlineStr">
         <is>
           <t>['Toss cucumbers in a large bowl with vinegar, sugar, red pepper flakes, and 2 tsp. salt. Chill, tossing once, at least 1 hour and up to 6 hours.', 'Just before serving, add dill and lemon juice and toss to combine. Taste and season with more salt if needed.']</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="F31" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/5bec46ad77ffda5e6a77f461/16:9/w_940,c_limit/spicy-lightly-pickled-cucumbers.jpg</t>
         </is>
@@ -1211,15 +1366,20 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
+          <t>Consider this recipe a no-brainer formula where you can sub in any raw veg, oil, or cheese you feel like. And if you’re feeling fancy, add some crunch (nuts, seeds, or fried onions) or herbs. Your new favorite side dish of summer!</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
           <t>['2 small Chioggia (candy-stripe) beets, trimmed, peeled', '2 Persian cucumbers', '1 medium watermelon radish, trimmed', '1 ounce Parmesan, Pecorino, Asiago, or other hard cheese, shaved', '1 lemon', 'Olive oil (for drizzling)', 'Flaky sea salt', 'Freshly ground black pepper']</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="E32" t="inlineStr">
         <is>
           <t>['Very thinly slice beets, cucumbers, and radish on a mandoline or with a knife. Arrange slices on a platter. Scatter cheese on top. Finely grate some lemon zest over salad, then slice open lemon and squeeze on some juice. Drizzle with oil; season with salt and pepper.']</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
+      <c r="F32" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a626a5df40d137127062a/16:9/w_940,c_limit/crunchy-salty-lemony-salad.jpg</t>
         </is>
@@ -1238,15 +1398,20 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
+          <t>A hard sear on the first side of the chicken ensures that it will get nicely browned without getting dry.</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
           <t>['2 large skinless, boneless chicken breasts (about 8 ounces each)', 'Kosher salt, freshly ground pepper', '5 tablespoons olive oil, divided', '½ small head of cabbage, very thinly sliced (about 4 cups)', '½ small red onion, very thinly sliced', '½ teaspoon crushed red pepper flakes', '2 tablespoons red wine vinegar']</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="E33" t="inlineStr">
         <is>
           <t>['Pound chicken between 2 sheets of plastic wrap to ¼" thick; season with salt and pepper. Heat 1 Tbsp. oil in large skillet over high. Carefully place 1 chicken breast in skillet (laying it away from you) and cook until golden brown and nearly cooked through, about 3 minutes. Turn and cook until cooked through, about 1 minute (second side will not brown). Transfer to a large plate. Repeat with 1 Tbsp. oil and remaining cutlet. Let the cutlets rest while you make the slaw.', 'Toss cabbage, onion, and red pepper flakes in a medium bowl; season with salt. Drizzle in vinegar and remaining 3 Tbsp. oil and toss again.', 'Top cutlets with slaw.']</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
+      <c r="F33" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a63002b659b48a371c336/16:9/w_940,c_limit/chicken-paillards-with-red-cabbage-and-onion-slaw.jpg</t>
         </is>
@@ -1265,15 +1430,20 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
+          <t>Think of this like a BLT minus the splattering bacon grease. With each bite you get that ideal combo of ingredients—sweet tomato, rich egg, crisp iceberg lettuce. You just need to get every element right. A nine-minute egg (so its center is just a touch tender), the ripest heirloom or beefsteak, basic iceberg, plenty of mayo, and the squishiest white bread you can find (griddled for extra credit). Oh, and don't forget plenty of salt and pepper on the egg and the tomato.</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
           <t>['2 slices white sandwich bread', '¼ cup Hellmann’s or Best Foods mayonnaise, divided', '2 thick ripe beefsteak tomato slices', 'Kosher salt, freshly ground pepper', '2 hard-boiled eggs, peeled, sliced crosswise', '3 leaves iceberg lettuce']</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="E34" t="inlineStr">
         <is>
           <t>['Spread both sides of bread slices all the way to the edges with the thinnest layer of mayonnaise possible. Heat a dry large skillet over medium-low; cook bread until golden, about 3 minutes per side. Transfer to a plate; let cool. Spread remaining mayonnaise over both slices of bread. Top a slice with tomatoes; season generously with salt and pepper. Arrange eggs over tomatoes; season. Top with lettuce, close sandwich, and cut in half.']</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="F34" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a65b67654ad34116652c8/16:9/w_940,c_limit/ELT.jpg</t>
         </is>
@@ -1292,15 +1462,20 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
+          <t>Mature bok choy has the same sweet and mild flavor of the baby stuff but is much easier to cook on the grill—and you’ll get a better yield, too.</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
           <t>['1 tablespoon olive oil, plus more for grill and drizzling', '½ cup unsweetened coconut flakes', '1 lime', '4 5–6-ounce skinless, boneless halibut fillets', 'Kosher salt, freshly ground pepper', '1 small head of bok choy, leaves separated, thick stems trimmed', '¾ cup unsweetened coconut milk']</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="E35" t="inlineStr">
         <is>
           <t>['Prepare a grill for medium heat; oil grate. Pulse coconut flakes in a food processor or a blender until coarsely chopped. Finely grate lime zest directly onto halibut and pack on coconut flakes. Drizzle lightly with oil; season with salt and pepper. Lightly coat bok choy with 1 Tbsp. oil; season with salt. Grill halibut, turning once, until browned on both sides and just opaque in center, about 5 minutes.', 'Meanwhile, grill bok choy leaves until lightly browned and tender, about 30 seconds per side.', 'Squeeze 2 Tbsp. lime juice into a small bowl and stir in coconut milk; season dressing with salt.', 'Divide halibut and bok choy among plates and drizzle with dressing.']</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
+      <c r="F35" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a58b75df40d1371270626/16:9/w_940,c_limit/grilled-halibut-and-bok-choy-with-coconut-lime-dressing.jpg</t>
         </is>
@@ -1319,15 +1494,20 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
+          <t>Set a large colander in the sink before you add the shrimp so you can drain the boil as soon as it comes off the heat.</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
           <t>['2 pounds small red-skinned potatoes', '¼ cup Zatarain’s Crawfish, Shrimp &amp; Crab Boil or Old Bay Seasoning, plus more for serving', 'Kosher salt', '2 lemons, divided', '4 ears of corn, husked, each ear cut crosswise into quarters', '2 pounds shell-on large shrimp, cut along back of shell, deveined', 'Olive oil (for drizzling)']</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="E36" t="inlineStr">
         <is>
           <t>['Combine potatoes, ¼ cup Zatarain’s, several large pinches of salt, and 5 quarts water in a large stockpot. Cut 1 lemon in half crosswise and squeeze juice into pot, then toss in halves. Bring to a boil, reduce heat, and simmer, uncovered, until potatoes are fork-tender, 20–25 minutes.', 'Add corn to pot; increase heat to high and bring liquid back to a boil. Add shrimp, cover pot, and turn off heat. Poach shrimp until just cooked through, about 2 minutes. Immediately pour entire contents of pot into a large colander to drain, then spread out corn, potatoes, and shrimp on a large rimmed baking sheet or sheets of newspaper; discard lemon halves. Sprinkle with more Zatarain’s and drizzle with oil. Cut remaining lemon into wedges and serve alongside for squeezing over.']</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
+      <c r="F36" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a66747654ad34116652ca/16:9/w_940,c_limit/no-frills-shrimp-boil.jpg</t>
         </is>
@@ -1346,15 +1526,20 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
+          <t>Old Tom gin is a revival of a type of gin that was popular in 18th-century England and is trendy again. Its botanicals enhance the peach flavor. You should be able to find it at most well-stocked liquor stores. This recipe is from bartender Dorothy Elizabeth at Standby in Detroit, MI.</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
           <t>['1 sprig thyme or lemon thyme', '½ ripe peach, sliced into thin wedges, divided', '1 ounce Old Tom gin', 'Club soda']</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
+      <c r="E37" t="inlineStr">
         <is>
           <t>['Muddle thyme sprig and all but 1 of the peach wedges in a highball glass (peaches should be smashed to a pulp). Fill glass partway with ice and add gin. Stir vigorously, then fill glass with ice and top off cocktail with club soda. Garnish with reserved peach wedge.']</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
+      <c r="F37" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a67bcb85671732e0d5584/16:9/w_940,c_limit/feeling-peachy.jpg</t>
         </is>
@@ -1373,15 +1558,20 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
+          <t>Kitchen economy: Use any leftover cooked vegetables, grains, or herbs in your fridge for this frittata, then use any leftover frittata for a sandwich the next day.</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
           <t>['6 large eggs', '6 ounces leftover roasted vegetables, cut into ½-inch pieces (about 1½ cups)', '½ cup leftover cooked grains', '1 ounce coarsely grated or crumbled cheese', '1 tablespoon finely chopped tender herbs, such as thyme, basil, and/or chives', 'Kosher salt', 'Freshly ground black pepper', '2 tablespoons extra-virgin olive oil, divided']</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="E38" t="inlineStr">
         <is>
           <t>['Vigorously whisk 6 eggs in a medium bowl until streak-free.HERE’S HOW TO BUY THE BEST EGGS POSSIBLE.', 'Add 5 oz. vegetables, ½ cup grains, 1 oz. grated cheese, and 1 Tbsp. herbs; season with salt and pepper. Mix with a rubber spatula to combine.', 'Heat 1 Tbsp. oil in a medium nonstick skillet over medium; swirl skillet to coat with oil.', 'Add egg mixture and cook until edges are set, about 30 seconds.', 'Using spatula, agitate eggs by scraping bottom of skillet in a small circular motion and bringing edges toward center of pan to form large curds, then let mixture sit undisturbed until edges are set again, about 1 minute.', 'Reduce heat to low and continue to cook, tilting skillet and lifting edges up with spatula to allow uncooked egg to flow underneath and around sides, until surface is wet but center is mostly set when you shake the pan, about 5 minutes.', 'Shake skillet to loosen frittata. Place a large plate over skillet and invert frittata onto plate.', 'Heat remaining 1 Tbsp. oil in skillet over medium, swirling to coat. Slide frittata back into skillet; reduce heat to low. Cook until set all the way through, about 3 minutes.', 'Let frittata cool in skillet 5 minutes, then invert onto a cutting board.', 'Season frittata with salt and pepper. Cut into wedges to serve.', 'Do Ahead: Frittata can be made 1 day ahead. Cover and chill. Bring to room temperature before serving.']</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
+      <c r="F38" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/5a3831db9c6db03fdcaf229f/3:2/w_940,c_limit/use-it-up-fritatta-16x9.jpg</t>
         </is>
@@ -1400,15 +1590,20 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
+          <t>Technically, pesto should be pounded or processed to a paste, but sometimes shortcuts pay off. This chopped version yields a more varied texture and requires nothing more than a cutting board and a knife.</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
           <t>['½ cup walnuts', '1 garlic clove', 'Kosher salt', '1½ ounces aged Gouda or Parmesan, grated on the small holes of a box grater (about 1 cup), plus more for serving', '2 cups basil leaves', '½ cup olive oil, plus more for serving', 'Freshly ground black pepper', '12 ounces dried short ruffled or corkscrew pasta (such as fusilli, gemelli, or campanelle)']</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
+      <c r="E39" t="inlineStr">
         <is>
           <t>['Preheat oven to 350°. Toast walnuts on a rimmed baking sheet, tossing once, until golden brown, 8–10 minutes. Let cool.', 'Meanwhile, smash garlic under the flat side of a chef’s knife in the center of your cutting board. Add a couple of pinches of salt and continue smashing with the side of your knife until garlic and salt form a paste. Scatter toasted nuts over garlic and smash nuts with the flat side of your knife to break into small bits. Sprinkle cheese over nuts and chop until nuts and cheese are the texture of fine breadcrumbs. Transfer to a large bowl. Finely chop basil and add to bowl with nut mixture. Stir in ½ cup oil and season generously with salt and pepper.', 'Cook pasta in a large pot of boiling salted water, stirring occasionally, until al dente. Drain, reserving about ½ cup pasta cooking liquid.', 'Add hot pasta to bowl with pesto and toss thoroughly to combine. If pasta seems dry, add a splash of pasta cooking liquid to moisten. Taste and season with more salt if needed.', 'Top pasta with more grated cheese and drizzle with a little oil.', 'Do Ahead: Pesto can be made 3 hours ahead. Pour oil over top instead of stirring into pesto. Store airtight at room temperature.']</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
+      <c r="F39" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a8d657102712b68401ab2/16:9/w_940,c_limit/pasta-with-chopped-pesto.jpg</t>
         </is>
@@ -1427,15 +1622,20 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
+          <t>Skirt steak is the ultimate summer steak for grilling—quick cooking, buttery, and versatile.</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
           <t>['3 tablespoons gochujang (Korean hot pepper paste), plus more for serving', '3 tablespoons olive oil, plus more for grill', '3 tablespoons plus ½ cup seasoned rice vinegar', 'Kosher salt', '1 medium red onion, halved through root end', '1 skirt steak (about 1 pound), halved crosswise', 'Warm tortillas (for serving)']</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="E40" t="inlineStr">
         <is>
           <t>['Combine 3 Tbsp. gochujang, 3 Tbsp. oil, and 3 Tbsp. vinegar in a large resealable plastic bag. Throw in several generous pinches of salt and grate in half of onion on the large holes of a box grater. Add steak and seal bag, pressing out air, then rub steak to coat; chill at least 30 minutes and up to 12 hours.', 'Meanwhile, thinly slice remaining half of onion and combine in a large bowl with remaining ½ cup vinegar and a pinch of salt. Let sit until onion is softened, at least 30 minutes and up to 2 hours; drain.', 'Prepare a grill for medium-high heat; oil grate. Remove steak from bag, letting excess marinade drip off; discard marinade. Grill, turning once or twice, until lightly charred on the outside and medium-rare in the thickest part, 4–6 minutes, depending on the thickness of the meat. Transfer to a cutting board and let rest 10 minutes before thinly slicing against the grain.', 'Season meat with more salt and serve with tortillas, pickled onion, and more gochujang.']</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
+      <c r="F40" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a8eaab85671732e0d558a/16:9/w_940,c_limit/gochujang-marinated-skirt-steak.jpg</t>
         </is>
@@ -1454,15 +1654,20 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
+          <t>Also known as Fava in Greek cuisine, this herby and bright purée recipe could also be made with nearly any other pulse or bean. It's often served alongside fish or as part of a meze spread.</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
           <t>['1 small onion, finely chopped', '1 cup yellow or red lentils', '1 teaspoon ground cumin', 'Kosher salt, freshly ground pepper', '1 cup cilantro leaves with tender stems, plus more for serving', '¼ cup olive oil, plus more for drizzling', '2 tablespoons fresh lime juice, plus more for serving']</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="E41" t="inlineStr">
         <is>
           <t>['Combine onion, lentils, cumin, and 4 cups water in a medium saucepan; season with salt and pepper. Bring to a boil, reduce heat to medium-low, and simmer until lentils are falling-apart tender, 25–30 minutes. Let cool.', 'Purée lentil mixture, 1 cup cilantro, ¼ cup oil, and 2 Tbsp. lime juice in a blender until smooth; season with salt and pepper. Spoon into a bowl. Drizzle with oil and lime juice; top with more cilantro.', 'Do Ahead: Lentil purée can be made 1 day ahead; cover and chill. Bring to room temperature before serving.']</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
+      <c r="F41" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a81cab85671732e0d5586/16:9/w_940,c_limit/lentil-puree-with-cilantro.jpg</t>
         </is>
@@ -1481,15 +1686,20 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
+          <t>If you are on the fence about cinnamon in savory dishes, this could be the chicken recipe that puts it in your YES column.</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
           <t>['4 chicken legs (thigh and drumstick)', 'Kosher salt, freshly ground pepper', '2 tablespoons olive oil', '2 small onions, thinly sliced', '2 pounds mixed tomatoes, cut into wedges if large', '3 3-inch cinnamon sticks', '1 tablespoon fresh lemon juice', 'Lemon wedges (for serving)']</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
+      <c r="E42" t="inlineStr">
         <is>
           <t>['Season chicken generously with salt and pepper. Heat oil in a medium Dutch oven or heavy shallow pot over medium-high. Cook chicken, skin side down, reducing heat as needed to avoid scorching, until skin is deep golden brown, 10–12 minutes. Transfer to a plate.', 'Reduce heat to medium and add onions to same pot. Cook, stirring occasionally, until very soft and just beginning to brown around the edges, 8–10 minutes. Add tomatoes and cinnamon sticks. Cook, stirring occasionally, until tomatoes are softened and juices have thickened slightly, 6–8 minutes. Return chicken to pot, arranging skin side up. Cover pot, reduce heat to low, and simmer gently until chicken is cooked through, 45–60 minutes.', 'Uncover pot and continue to simmer until juices are thickened and meat is close to falling off the bone, 45–60 minutes. Add lemon juice; taste and season with more salt and pepper as needed. Serve with lemon wedges.', 'Do Ahead: Chicken can be braised 3 days ahead. Let cool in liquid; cover and chill. Reheat gently before serving.']</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr">
+      <c r="F42" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a82e72b659b48a371c338/16:9/w_940,c_limit/braised-chicken-and-tomatoes.jpg</t>
         </is>
@@ -1508,15 +1718,20 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
+          <t>If you can only find skin-on halibut, carry on: After the fish is cooked, wiggle a spatula between the skin and the fillet, and it will slip right off.</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
           <t>['¼ cup olive oil, plus more for grill and drizzling', '1 lime', '4 5–6-ounce skinless, boneless halibut fillets', 'Kosher salt, freshly ground pepper', '2 medium zucchini', '¼ cup coarsely chopped unsalted, roasted pumpkin seeds (pepitas)', '½ cup coarsely chopped cilantro, plus more for serving']</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="E43" t="inlineStr">
         <is>
           <t>['Prepare a grill for medium heat; oil grates. Finely grate lime zest directly onto halibut and lightly drizzle with oil; season with salt and pepper. Lightly coat zucchini with oil and season with salt. Grill halibut, turning once, until browned on both sides and just opaque in the center, about 5 minutes.', 'Meanwhile, grill zucchini just until lightly charred on all sides but still basically raw, about 5 minutes.', 'Combine pumpkin seeds and ¼ cup oil in a small bowl; squeeze in 2 Tbsp. juice from lime and toss to combine. Season with salt and pepper and mix in ½ cup cilantro.', 'Thinly slice zucchini into ribbons on a mandoline. Divide among plates and set halibut on top. Spoon pumpkin seed mixture over; top with more cilantro.']</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr">
+      <c r="F43" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a57876c75df51bc0b91f4/16:9/w_940,c_limit/grilled-halibut-and-summer-squash-with-pumpkin-seeds.jpg</t>
         </is>
@@ -1535,15 +1750,20 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
+          <t>Steaming the apricots over the rice while it rests softens them just enough.</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
           <t>['1 cup skin-on almonds', '1 tablespoon olive oil', 'Kosher salt', '1 cup basmati rice', '1 3x1-inch strip lemon zest', '⅓ cup chopped dried apricots', '2 cups chopped parsley', '1 tablespoon fresh lemon juice']</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="E44" t="inlineStr">
         <is>
           <t>['Preheat oven to 300°. Toss almonds with oil on a small rimmed baking sheet; season with salt. Roast, tossing occasionally, until golden brown, 10–12 minutes. Let cool, then chop.', 'Meanwhile, rinse rice in several changes of water until water runs clear. Bring rice, lemon zest, and 1½ cups water to a boil in a small saucepan; season with salt. Reduce heat, cover pan, and simmer until rice is tender, 18–20 minutes. Remove from heat, uncover, and scatter apricots over rice. Cover; let sit 10 minutes. Fluff rice with a fork, then mix in almonds, parsley, and lemon juice. Taste and season with more salt if needed.']</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
+      <c r="F44" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a866d7654ad34116652ce/16:9/w_940,c_limit/rice-with-parsley-almonds-and-apricots.jpg</t>
         </is>
@@ -1562,15 +1782,20 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
+          <t>Soaking and squeezing the bread softens it so that it can combine much more easily with the meat.</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
           <t>['1 small onion', '3 1-inch-thick slices stale white sandwich bread, crusts removed (about 4 ounces)', '2 large eggs, beaten to blend', '1 pound ground beef chuck (20% fat)', '1 cup finely chopped mint', 'Kosher salt, freshly ground pepper', '1 cup olive oil', 'Tzatziki (for serving)']</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
+      <c r="E45" t="inlineStr">
         <is>
           <t>['Grate onion on the large holes of a box grater and squeeze firmly with your hands to release excess liquid. Place onion in a medium bowl.', 'Working one at a time, hold slices of bread under running water very briefly to soften (be careful not to waterlog or make soggy). Squeeze firmly with your hands to expel the water. Very finely chop bread and place in bowl with onion. Add eggs and mix well. Add beef and mint; season generously with salt and pepper. Mix with your hands until evenly distributed; be careful not to overwork. Portion into 24 balls (about 1 heaping Tbsp. each).', 'Heat oil in a medium skillet, preferably cast iron, over medium. Working in 2 batches, add meatballs and press down on each one to flatten slightly. Fry until browned and very crisp, about 3 minutes. Turn and fry on other side until browned and very crisp, about 3 minutes. Transfer to a platter as you work. Serve with Tzatziki.', 'Do Ahead: Meatballs can be formed 1 day ahead. Cover and chill.']</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr">
+      <c r="F45" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a84077102712b68401aae/16:9/w_940,c_limit/meatballs-with-mint.jpg</t>
         </is>
@@ -1589,15 +1814,20 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
+          <t>Keeping the garlic whole and removing once it has added enough flavor will keep the flavor more mild, but if you want more of a punch, grate it before adding and leave it in. Serve alongside Meatballs and Mint.</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
           <t>['3 Persian or ½ English hothouse cucumbers, cut into ¼-inch pieces', 'Kosher salt', '1 cup plain whole-milk Greek yogurt', '3 tablespoons olive oil', '2 tablespoons fresh lemon juice', '1 garlic clove, lightly crushed', '¼ cup chopped mint']</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
+      <c r="E46" t="inlineStr">
         <is>
           <t>['Toss cucumbers with a few generous pinches of salt in a small bowl; firmly squeeze several times with your hands to release excess water. Drain.', 'Mix cucumbers, yogurt, oil, lemon juice, and garlic in a medium bowl; season with salt. Let sit at room temperature until tzatziki tastes garlicky, 15–20 minutes; discard garlic. Stir in mint just before serving.', 'Do Ahead: Tzatziki (without mint) can be made 3 days ahead. Cover and chill.']</t>
         </is>
       </c>
-      <c r="E46" t="inlineStr">
+      <c r="F46" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a857a2b659b48a371c33a/16:9/w_940,c_limit/tzatziki.jpg</t>
         </is>
@@ -1616,15 +1846,20 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
+          <t>Don’t believe the hype that every vinaigrette recipe should have one part acid to three parts oil. This more assertive ratio brings a lot more flavor to the table. Serve with Mixed Greens with Yogurt Dressing and Dill, Tomato Salad with Feta and Pistachios and Shaved Radish Salad with Walnuts and Mint.</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
           <t>['⅔ cup olive oil', '⅓ cup fresh lemon juice', 'Kosher salt, freshly ground pepper']</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
+      <c r="E47" t="inlineStr">
         <is>
           <t>['Whisk oil and lemon juice in a small bowl or shake in a resealable jar to emulsify; season with salt and pepper.']</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr">
+      <c r="F47" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a87505df40d137127062e/16:9/w_940,c_limit/basic-lemon-vinaigrette.jpg</t>
         </is>
@@ -1643,15 +1878,20 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
+          <t>A couple tablespoons of yogurt miraculously transform a basic vinaigrette recipe into a new creamy dressing.</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
           <t>['¼ cup Basic Lemon Vinaigrette', '2 tablespoons plain whole-milk Greek yogurt', '8 cups mixed tender greens (such as mizuna and baby lettuces)', '¼ cup coarsely chopped dill', '2 tablespoons toasted sesame seeds', 'Kosher salt, freshly ground pepper']</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
+      <c r="E48" t="inlineStr">
         <is>
           <t>['Whisk vinaigrette and yogurt in a large bowl. Add greens, dill, and sesame seeds and toss to coat; season salad with salt and pepper.']</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr">
+      <c r="F48" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a884f7654ad34116652d0/16:9/w_940,c_limit/mixed-greens-with-yogurt-dressing.jpg</t>
         </is>
@@ -1670,15 +1910,20 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
+          <t>Serve this salad as soon as it is assembled so all of the tomato juices and flavor stay where they belong.</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
           <t>['3 tablespoons pistachios', '1 pound mixed tomatoes, some sliced, some cut into wedges', 'Kosher salt, freshly ground pepper', '¼ cup Basic Lemon Vinaigrette', '¼ cup chopped parsley, plus leaves for serving', '¼ cup crumbled feta']</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
+      <c r="E49" t="inlineStr">
         <is>
           <t>['Preheat oven to 350°. Toast pistachios on a rimmed baking sheet, tossing once, until golden brown, 6–8 minutes. Let cool, then chop.', 'Arrange tomatoes on a plate; season lightly with salt and pepper. Mix vinaigrette, ¼ cup parsley, and two-thirds of pistachios in a small bowl. Drizzle over tomatoes. Top with feta, parsley leaves, and remaining pistachios.']</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr">
+      <c r="F49" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a896d7102712b68401ab0/16:9/w_940,c_limit/tomato-salad-with-feta-and-pistachios.jpg</t>
         </is>
@@ -1697,15 +1942,20 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
+          <t>Mandolines were made for recipes like this; even slices will make this simple salad look like the work of a pro.</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
           <t>['¼ cup walnuts', '2 cups thinly sliced mixed radishes', 'Flaky sea salt', 'Freshly ground black pepper', '¼ cup Basic Lemon Vinaigrette', '2 tablespoons mint leaves']</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
+      <c r="E50" t="inlineStr">
         <is>
           <t>['Preheat oven to 350°. Toast walnuts on a rimmed baking sheet, tossing once, until golden brown, 8–10 minutes. Let cool; crush with the flat side of a chef’s knife.', 'Arrange radishes on a plate. Lightly season with salt and pepper and drizzle vinaigrette over; top with walnuts and mint.']</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr">
+      <c r="F50" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a8a6db85671732e0d5588/16:9/w_940,c_limit/shaved-radish-salad-with-walnuts-and-mint.jpg</t>
         </is>
@@ -1724,15 +1974,20 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
+          <t>We usually rail against kitchen tools that do only one thing and take up precious drawer space, but cherry pitters earn their keep as far as we are concerned.</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
           <t>['1 pound fresh cherries, pits removed', '⅓ cup fresh red currants or three 3x1-inch strips lemon zest', '3 tablespoons sugar', '1½ cups plain whole-milk Greek yogurt', '3 tablespoons wildflower or thyme honey', 'Pinch of kosher salt']</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
+      <c r="E51" t="inlineStr">
         <is>
           <t>['Bring cherries, currants, and sugar to a simmer in a medium saucepan over medium heat. Cook until fruit is tender and juices are thick enough to coat a spoon, 8–12 minutes. (Fish out lemon zest if using.)', 'Mix yogurt, honey, and salt in a small bowl. Scoop into bowls; top with compote.']</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr">
+      <c r="F51" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a8ba05df40d1371270630/16:9/w_940,c_limit/cherry-compote-with-honey-yogurt.jpg</t>
         </is>
@@ -1751,15 +2006,20 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
+          <t>Real talk: This is a dish to make when the tomatoes are peaking—at the farmers’ market, you should be able to smell them before you see them. The moment only comes around once a year, so make the most of it (which is to say, do very little with them). This is part of BA's Best, a collection of our essential recipes.</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
           <t>['1 pint mixed cherry tomatoes, preferably heirloom, halved', '7 tablespoons (or more) extra-virgin olive oil, divided', 'Flaky sea salt', '2 pounds mixed medium and large tomatoes, preferably heirloom, cut into thin slices and/or wedges', '8 ounces buffalo mozzarella or mozzarella, room temperature, torn into pieces', 'Coarsely ground black pepper', 'Small basil leaves and toasted country bread (for serving)']</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr">
+      <c r="E52" t="inlineStr">
         <is>
           <t>['Toss cherry tomatoes with 1 Tbsp. oil in a small bowl; season with salt.', 'Arrange tomato slices on a platter, slightly overlapping; season generously with salt. Arrange mozzarella over tomatoes; lightly season mozzarella with salt. Spoon cherry tomatoes over salad and drizzle with 6 Tbsp. oil; season with pepper. Let stand 30 minutes to let flavors meld and release juices from tomatoes and mozzarella.', 'Top salad with basil and additional salt and oil, if desired. Serve with bread alongside.']</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr">
+      <c r="F52" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596cdb0d7102712b68401ae0/16:9/w_940,c_limit/ultimate-caprese-salad.jpg</t>
         </is>
@@ -1778,15 +2038,20 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
+          <t>Cooking the peppers for only a short time preserves their green color and means they’ll bring some bite and texture to the salsa.</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
           <t>['3 1½-inch-thick boneless rib eyes (about 1¼ pounds each)', 'Kosher salt, freshly ground pepper', '1¼ cups olive oil, divided', '1 pound shishito peppers', '2 garlic cloves, finely grated', '¼ cup sherry vinegar or red wine vinegar', 'Flaky sea salt']</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr">
+      <c r="E53" t="inlineStr">
         <is>
           <t>['The night before you plan to cook the steaks, pat dry with paper towels and set on a wire rack set inside a rimmed baking sheet. Season generously with kosher salt and pepper and chill, uncovered, until about 1 hour before grilling. (If you don’t have time, skipping the overnight chill is fine.) Let steaks come to room temperature.', 'Prepare a grill for medium-high, indirect heat (for a charcoal grill, bank coals on one side of grill; for a gas grill, leave one or two burners off). Grill steaks over direct heat, turning once, until nicely charred, about 4 minutes per side. Move steaks over indirect heat and continue grilling, turning halfway through, until browned all over, about 4 minutes per side. Using tongs, hold a steak perpendicular to grill and sear bone side and fat-cap side to render some of the fat, about 2 minutes per side. Repeat with remaining steaks. Insert an instant-read thermometer into the thickest part of each steak; if it registers 120° for rare (steaks will carry over to 125°, or medium-rare, as they rest), they’re done. If they’re not quite there, continue to cook over indirect heat—another 2–4 minutes should do it. Transfer to a cutting board and let rest 20 minutes before slicing against the grain.', 'Meanwhile, heat ¼ cup oil in a large skillet, preferably cast iron, over high heat. As soon as oil starts to smoke, add peppers to cover bottom of pan in a single layer (don’t crowd). Cook, tossing occasionally, until blistered in spots but still green, about 3 minutes. (You don’t want them to collapse or soften too much.) Transfer to another cutting board and repeat with remaining peppers. Let sit until cool enough to touch. Coarsely chop peppers and place in a small bowl. Mix in garlic, vinegar, and remaining 1 cup oil; season with kosher salt.', 'Transfer steaks to a platter and spoon shishito pepper salsa over top; sprinkle with sea salt.', 'Do Ahead: Salsa can be made 8 hours ahead. Cover and chill.']</t>
         </is>
       </c>
-      <c r="E53" t="inlineStr">
+      <c r="F53" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596cd3dcb85671732e0d55af/16:9/w_940,c_limit/grilled-rib-eye-with-shishito-pepper-salsa.jpg</t>
         </is>
@@ -1805,15 +2070,20 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
+          <t>The longer you let these birds soak up the beer, spices, and orange, the better.</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
           <t>['2 3½–4-pound chickens, backbones removed', '3 oranges, divided', '4 12-ounce bottles lager', '6 tablespoons kosher salt, plus more', '3 tablespoons Aleppo-style pepper or other mild crushed pepper, plus more for serving', '3 tablespoons sumac, plus more for serving', 'Sumac can be found at Middle Eastern markets, specialty foods stores, and online.']</t>
         </is>
       </c>
-      <c r="D54" t="inlineStr">
+      <c r="E54" t="inlineStr">
         <is>
           <t>['Place one of the chickens on a work surface, skin side up. Using your palms, press firmly on breastbone to flatten breast (you should hear the bone crack). Repeat with remaining chicken.', 'Slice 2 oranges into ½"-thick rounds and squeeze juice from slices into a tall pot; drop in slices and add beer, 6 Tbsp. salt, 3 Tbsp. Aleppo-style pepper, and 3 Tbsp. sumac. Submerge chickens in marinade and turn to coat. Weigh down with a plate and chill at least 2 hours and up to 12 hours.', 'Place a rack in upper third of oven; preheat to 475°. Remove chickens from marinade; discard marinade. Pat chickens dry with paper towels and season generously with salt. Place side by side on a wire rack set inside a rimmed baking sheet. Roast, rotating baking sheet halfway through, until an instant-read thermometer inserted into the thickest part of thighs registers 165°, 35–40 minutes. Transfer chickens to a cutting board and let rest at least 10 minutes.', 'Slice half of the remaining orange into ¼”-thick rounds, then cut the other half into wedges. Transfer chickens to a platter, scatter orange slices and wedges over, and sprinkle with more Aleppo-style pepper and sumac. Dip some wedges in spices if desired.']</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr">
+      <c r="F54" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596cd4d62b659b48a371c35e/16:9/w_940,c_limit/beer-and-orange-marinated-roast-chicken.jpg</t>
         </is>
@@ -1832,15 +2102,20 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
+          <t>Buckwheat adds a unique flavor to this salad, but other grains, such as cooked barley, farro, or bulgur, would be good too.</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
           <t>['⅓ cup olive oil, plus more for drizzling', '1½ cups buckwheat groats', '2 lemons', '8 ounces shiitake mushrooms, thinly sliced', '3 cups parsley leaves with tender stems (about 1 large bunch)', '4 ounces goat’s- or cow’s-milk Gouda, shaved, divided', 'Kosher salt, freshly ground pepper']</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr">
+      <c r="E55" t="inlineStr">
         <is>
           <t>['Heat ⅓ cup oil in a large skillet over medium-high. Cook buckwheat, stirring often, until slightly darkened in color and fragrant, about 5 minutes; transfer buckwheat and oil to a large bowl.', 'While the buckwheat cools, cut peels and white pith from lemons; discard. Cut between membranes to release segments onto a cutting board. Squeeze membranes over a small bowl to yield ¼ cup juice; discard membranes. Coarsely chop segments and add to bowl with buckwheat. Add lemon juice, mushrooms, parsley, and half of Gouda and season with salt and pepper; toss to combine. Top with remaining Gouda and drizzle with oil. Grind a little more pepper on top.']</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr">
+      <c r="F55" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596ccdeeb85671732e0d55a8/16:9/w_940,c_limit/buckwheat-and-shiitake-mushroom-salad-with-gouda.jpg</t>
         </is>
@@ -1859,15 +2134,20 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
+          <t>This is a beautifully simple salad, which is why you should get your hands on plums from your local farmers’ market if you can.</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
           <t>['2 medium fennel bulbs', '6 small plums, halved, or 3 medium plums, quartered', '2 tablespoons Champagne vinegar or white wine vinegar', '2 tablespoons olive oil, plus more for drizzling', 'Kosher salt, freshly ground pepper']</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr">
+      <c r="E56" t="inlineStr">
         <is>
           <t>['Remove stalks and fronds from fennel bulbs. Cut fennel bulbs in half lengthwise and thinly slice on a mandoline; place in a large bowl. Remove fronds from stalks and set aside. Thinly slice stalks and add to bowl along with plums, vinegar, and 2 Tbsp. oil. Season with salt and pepper and toss well. Let salad sit 5 minutes.', 'Coarsely chop reserved fennel fronds; scatter over salad. Drizzle with more oil.']</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr">
+      <c r="F56" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596ccf6d5df40d1371270642/16:9/w_940,c_limit/shaved-fennel-salad-with-plums.jpg</t>
         </is>
@@ -1886,15 +2166,20 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
+          <t>Super-sweet pineapple? You may not need all of the sugar for this punch recipe.</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
           <t>['1 750-ml bottle Bacardí Superior Rum', '1½ cups fresh pineapple juice', '1½ cups fresh ruby red grapefruit juice', '¾ cup (or more) sugar', '1 750-ml bottle chilled sparkling rosé', '4–6 pineapples (optional)', 'Grapefruit wedges (for serving)']</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
+      <c r="E57" t="inlineStr">
         <is>
           <t>['Whisk rum, pineapple juice, grapefruit juice, and sugar in a pitcher or large bowl until sugar is dissolved. Chill until cold, at least 1 hour and up to 4 hours. Stir in rosé. Taste and add more sugar, if desired.', 'If using pineapples, cut off fronds and set aside for serving. Cut a ¼"-thick slice off the bottoms and tops so they will sit upright and won’t wobble. Cut pineapples in half crosswise. Working with 1 half at a time, use a paring knife to cut away flesh ½" from skin. Using a large metal spoon, scoop out flesh, being careful not to pierce the skin. Save flesh for another use.', 'Ladle punch into ice-filled pineapple halves or rocks glasses and garnish each with a couple of pineapple leaves, if using, and a grapefruit wedge.']</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr">
+      <c r="F57" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a5c7cb85671732e0d5580/16:9/w_940,c_limit/varadero-cooler.jpg</t>
         </is>
@@ -1913,15 +2198,20 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
+          <t>This sauce tastes like a cross between ranch and Alabama white sauce, which means you can basically put it on anything.</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
           <t>['1 cup mayonnaise', '½ cup evaporated milk', '1 garlic clove, finely grated', 'Kosher salt, freshly ground pepper', '3 pounds mixed heirloom tomatoes, cut into 1½-inch pieces', '1 tablespoon oregano leaves']</t>
         </is>
       </c>
-      <c r="D58" t="inlineStr">
+      <c r="E58" t="inlineStr">
         <is>
           <t>['Whisk mayonnaise, evaporated milk, garlic, a big pinch of salt, and a few grinds of pepper in a medium bowl. (It should be the consistency of pancake batter.)', 'Toss tomatoes with a big pinch of salt in a large bowl, then transfer to a platter. Drizzle sauce over to your liking (you don’t need to use all of it) and top with oregano. Grind more pepper over.', 'Do Ahead: White sauce can be made 1 day ahead. Cover and chill.']</t>
         </is>
       </c>
-      <c r="E58" t="inlineStr">
+      <c r="F58" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596cd2d1b85671732e0d55ac/16:9/w_940,c_limit/tomatoes-with-garlicky-white-sauce-and-oregano.jpg</t>
         </is>
@@ -1940,15 +2230,20 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
+          <t>In this riff on the Spanish tapas pan con tomate, you want to make sure the bread is really crisped through.</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
           <t>['16 medium tomatillos (about 1½ pounds), husks removed, rinsed, quartered', '4 teaspoons kosher salt', '1 tablespoon sugar', '1 ciabatta loaf', '3 tablespoons olive oil, plus more for drizzling', '2 garlic cloves, finely grated', '2 small green tomatoes, thinly sliced (optional)', 'Flaky sea salt']</t>
         </is>
       </c>
-      <c r="D59" t="inlineStr">
+      <c r="E59" t="inlineStr">
         <is>
           <t>['Toss tomatillos, kosher salt, and sugar in a small bowl. Gently massage until they feel soft and juicy. Cover and let sit at room temperature, tossing occasionally, until tomatillos have released some of their liquid, at least 4 hours and up to 12 hours.', 'Preheat oven to 300°. Holding a bread knife parallel to a cutting board, slice ciabatta in half. Slice each piece in half lengthwise, then cut each strip on a diagonal into about 4" pieces. Drizzle 3 Tbsp. oil over bread and rub each piece to evenly distribute oil. Place bread on a baking sheet and bake until browned all over and dried out and crisp, 60–75 minutes. Let cool.', 'Meanwhile, transfer tomatillos to a food processor; leave juices in bowl. Pulse until finely chopped but not smooth (mixture should look pulpy with bits of skin). Transfer to a medium bowl; add garlic.', 'Spoon tomatillo mixture over toast, then drizzle some of the reserved juices over. Top with green tomatoes, if using; drizzle with oil and sprinkle with sea salt.', 'Do Ahead: Tomatillo mixture can be made 1 day ahead. Cover and chill.']</t>
         </is>
       </c>
-      <c r="E59" t="inlineStr">
+      <c r="F59" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596cd62eb85671732e0d55b3/16:9/w_940,c_limit/pan-con-tomatillo.jpg</t>
         </is>
@@ -1967,15 +2262,20 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
+          <t>Smoked sablefish adds a bit of luxury to this easy scrambled eggs recipe. Swap in lox if it’s more readily available.</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
           <t>['4 tablespoons unsalted butter', '16 large eggs, beaten to blend', 'Kosher salt', '¾ cup crème fraîche, plus more for serving', '12 ounces smoked sablefish, sliced', '¼ small red onion, very thinly sliced', 'Freshly ground black pepper']</t>
         </is>
       </c>
-      <c r="D60" t="inlineStr">
+      <c r="E60" t="inlineStr">
         <is>
           <t>['Heat butter in a large nonstick skillet over medium-low. Once butter is foaming, add eggs and season with salt. Cook, stirring occasionally with a heatproof rubber spatula, until some curds begin to form, about 4 minutes. Mix in ¾ cup crème fraîche and cook, stirring occasionally, until eggs are barely set, about 3 minutes. Remove from heat and fold in sablefish.', 'Transfer eggs to a platter and spoon a few dollops of crème fraîche over. Top with onion and a few grinds of pepper.']</t>
         </is>
       </c>
-      <c r="E60" t="inlineStr">
+      <c r="F60" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596cd0697654ad341166530b/16:9/w_940,c_limit/soft-scrambled-eggs-with-sablefish-and-creme-fraiche.jpg</t>
         </is>
@@ -1994,15 +2294,20 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
+          <t>This recipe puts a spin on prosciutto and melon by swapping in smoked salmon for the salty dry-cured ham.</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
           <t>['1 2-pound honeydew melon', 'Olive oil (for drizzling)', 'Flaky sea salt', '8 ounces cold-smoked salmon, thinly sliced', 'Freshly ground black pepper', 'Coarsely chopped dill (for serving)']</t>
         </is>
       </c>
-      <c r="D61" t="inlineStr">
+      <c r="E61" t="inlineStr">
         <is>
           <t>['Slice off the top and bottom of the melon to create flat surfaces, then stand upright. Slice rind off melon in pieces; discard. Cut flesh in half through stem end; scoop out seeds and membrane from each half and set aside. Slice melon into ¾"-thick wedges; arrange on a platter.', 'Place reserved seeds and membrane in a fine-mesh sieve set over a small bowl and push out juice with a spoon; discard seeds and membrane. Drizzle melon juice over wedges, then drizzle with oil; season with salt. Drape smoked salmon on top. Drizzle with more oil and sprinkle with salt and pepper; top with dill.']</t>
         </is>
       </c>
-      <c r="E61" t="inlineStr">
+      <c r="F61" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596cd1802b659b48a371c35c/16:9/w_940,c_limit/honeydew-and-lox.jpg</t>
         </is>
@@ -2021,15 +2326,20 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
+          <t>Think of the cantaloupe as a two-for-one: It acts as a vessel while also being a bonus treat after you finish the granita.</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
           <t>['1 quart plain whole-milk Greek yogurt', '2 cups whole milk', '½ cup honey', 'Pinch of kosher salt', '4 very small cantaloupes (about 1½ pounds each)', '2 cups raspberries (about 1 pint)']</t>
         </is>
       </c>
-      <c r="D62" t="inlineStr">
+      <c r="E62" t="inlineStr">
         <is>
           <t>['Whisk yogurt, milk, honey, and salt in a large bowl to combine. Pour into a baking pan (metal works best). Freeze mixture until edges begin to set, about 30 minutes. Using a fork, scrape to break up frozen portions. Continue to freeze, scraping and breaking up frozen parts every 20–30 minutes, until mixture resembles fluffy shaved ice, 2–4 hours.', 'Cut cantaloupes in half crosswise and scrape out seeds; discard. Scoop some granita into each cantaloupe half; top with raspberries.', 'Do Ahead: Granita can be made 1 week ahead. Cover and keep frozen. Scrape to fluff just before serving.']</t>
         </is>
       </c>
-      <c r="E62" t="inlineStr">
+      <c r="F62" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596cd7b17654ad341166530d/16:9/w_940,c_limit/yogurt-granita-with-melon-and-raspberries.jpg</t>
         </is>
@@ -2048,15 +2358,20 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
+          <t>This recipe for waffles is crisp and delicate in an almost unreal way. Enjoy them hot off the iron with whipped cream and jam. Check out more in Magnus Nilsson's Nordic Cookbook.</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
           <t>['1¼ cups weak (soft) wheat flour (6½ ounces)', 'Generous pinch of kosher salt', 'Generous pinch of sugar', '1¼ cups cream', 'Melted unsalted butter (for brushing)']</t>
         </is>
       </c>
-      <c r="D63" t="inlineStr">
+      <c r="E63" t="inlineStr">
         <is>
           <t>['Pour ¾ cup + 1 Tbsp. water into a large bowl. Stir in flour, salt, and sugar to form a batter.', 'Using an electric mixer on medium-high speed, whip cream in another large bowl until soft peaks form; fold into batter (it should be fully combined, but not overmixed).', 'Heat waffle iron to proper working temperature and brush very lightly with butter. Pour in a suitable amount of batter and cook until waffle is nice and golden. Repeat with remaining batter.']</t>
         </is>
       </c>
-      <c r="E63" t="inlineStr">
+      <c r="F63" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/57accd5b1b334044149751d5/16:9/w_940,c_limit/Screen-Shot-2015-12-17-at-3.28.06-PM.png</t>
         </is>
@@ -2075,15 +2390,20 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
+          <t>Use the largest skillet you have (a straight-sided 12" is ideal) and a fish spatula for this fingerling potato recipe—the thin angled edge is just right for helping potatoes release from the skillet.</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
           <t>['3 pounds fingerling potatoes, scrubbed, halved lengthwise', '⅓ cup fresh lemon juice', '2 teaspoons kosher salt', '6 tablespoons unsalted butter, cut into pieces, divided', '⅓ cup chopped fresh parsley', 'Flaky sea salt']</t>
         </is>
       </c>
-      <c r="D64" t="inlineStr">
+      <c r="E64" t="inlineStr">
         <is>
           <t>['Combine potatoes, lemon juice, kosher salt, and 3 Tbsp. butter in a large straight-sided skillet or a Dutch oven; add cold water just to cover. Bring to a boil over medium-high heat and cook until potatoes are tender, 20–25 minutes. Increase heat and boil rapidly until pan is almost dry, 15–20 minutes more (there will still be a sheen of butterfat).', 'Using a slotted spoon, transfer about half of potatoes to a plate and arrange potatoes remaining in skillet cut side down in a single layer (if your skillet is smaller, you may need to work in a few batches). Reduce heat to medium and cook potatoes undisturbed until water is evaporated and cut sides of potatoes are deeply browned, 5–10 minutes.', 'Using a thin metal spatula, scrape skillet to cleanly release potatoes and transfer to a large bowl. Return skillet to medium heat, add 1 Tbsp. butter, and repeat browning process with reserved potatoes. After scraping skillet to release potatoes, return first batch, along with parsley and remaining 2 Tbsp. butter, to skillet and toss until potatoes are well coated. Serve sprinkled with sea salt.', 'Do Ahead: Potatoes can be boiled 4 hours ahead. Let cool in skillet, then cover and let sit at room temperature. Brown just before serving.']</t>
         </is>
       </c>
-      <c r="E64" t="inlineStr">
+      <c r="F64" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/57acd77053e63daf11a4da93/16:9/w_940,c_limit/lemon-and-parsley-skillet-roasted-fingerling-potatoes.jpg</t>
         </is>
@@ -2102,15 +2422,20 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
+          <t>If you’re feeling really decadent and fancy (as you should), add a splash of half-and-half or heavy cream just before serving. This is part of BA's Best, a collection of our essential recipes.</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
           <t>['3 tablespoons cocoa powder (preferably Dutch-processed), plus more for serving', '3 cups whole milk', '6 ounces semisweet chocolate (preferably Scharffen Berger), finely chopped', '3 tablespoons demerara or granulated sugar', 'Lightly sweetened whipped cream (for serving)']</t>
         </is>
       </c>
-      <c r="D65" t="inlineStr">
+      <c r="E65" t="inlineStr">
         <is>
           <t>['Bring ¾ cup water to a simmer in a medium saucepan over medium-high heat. Whisk in 3 Tbsp. cocoa powder until no lumps remain, then add milk and return to a simmer. Whisk in chocolate and sugar and cook, whisking frequently, until mixture is smooth and creamy and chocolate is melted, about 5 minutes.', 'Divide hot chocolate among mugs. Top with whipped cream and dust with cocoa powder.']</t>
         </is>
       </c>
-      <c r="E65" t="inlineStr">
+      <c r="F65" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/57accdd1f1c801a1038bc794/16:9/w_940,c_limit/Hot-Chocolate-2-of-5.jpg</t>
         </is>
@@ -2129,15 +2454,20 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
+          <t>This recipe would also work with small cipolline onions or larger torpedo-shaped shallots.</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
           <t>['2½ pounds shallots, peeled', '⅔ cup (or more) apple cider vinegar', '6 tablespoons unsalted butter', '¼ cup bourbon', '¼ cup pure maple syrup', '¼ teaspoon kosher salt, plus more', 'Freshly ground black pepper']</t>
         </is>
       </c>
-      <c r="D66" t="inlineStr">
+      <c r="E66" t="inlineStr">
         <is>
           <t>['Bring shallots, vinegar, butter, bourbon, maple syrup, ¼ tsp. salt, and 2 cups water to a boil in a large skillet over medium-high heat. Cover, reduce heat, and simmer, adding water by the tablespoonful if needed, until shallots are crisp-tender and liquid is partly evaporated, 25–30 minutes.', 'Uncover shallots and cook until liquid is evaporated and shallots begin to brown, about 5 minutes. Continue to cook, swirling pan often, until shallots and surface of skillet are covered in a rich brown caramel, about 6 minutes. Add ¼ cup water to skillet and stir to deglaze caramel and coat shallots. Season with salt and pepper. Transfer to a microwave-safe bowl and let cool.', 'To reheat, cover bowl with plastic wrap and microwave on high in 30-second intervals, tossing in between, until heated through, about 2 minutes. Taste and adjust seasoning with salt, pepper, and vinegar if needed.', 'Do Ahead: Shallots can be made 1 day ahead. Cover and chill.']</t>
         </is>
       </c>
-      <c r="E66" t="inlineStr">
+      <c r="F66" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/57acd8ce1b33404414975251/16:9/w_940,c_limit/cider-and-bourbon-glazed-shallots.jpg</t>
         </is>
@@ -2156,15 +2486,20 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
+          <t>There are two kinds of hash browns: The chunky, floury, vaguely brown but not crisp kind, and the lacy, crunchy, shredded version here. Guess which one we prefer? This is part of BA's Best, a collection of our essential recipes.</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
           <t>['½ cup (1 stick) unsalted butter or 6 tablespoons ghee', '3 russet potatoes (about 1½ pounds), peeled', 'Pinch of freshly ground black pepper', 'Pinch of cayenne pepper', '1 teaspoon kosher salt, plus more']</t>
         </is>
       </c>
-      <c r="D67" t="inlineStr">
+      <c r="E67" t="inlineStr">
         <is>
           <t>['Heat butter in a small saucepan over medium heat until foamy, about 3 minutes. Don’t let butter brown; reduce heat if needed. Skim off solids; discard. Using the coarse grater disk on a food processor or the largest holes on a box grater, shred potatoes. Transfer immediately to a large bowl of cold water; stir until water is cloudy. Drain and rinse potatoes well under cold running water to remove any excess starch, which can make hash browns gummy.', 'Transfer to a large kitchen towel. Gather together ends of towel and twist over sink, squeezing firmly to wring out as much liquid as possible (another step that ensures crisp results). Open towel and toss potatoes to loosen. Gather up towel and wring out potatoes once more. Transfer potatoes to a medium bowl and toss with pepper, cayenne, and 1 tsp. salt (make sure seasonings are evenly distributed).', 'Heat 4 Tbsp. clarified butter or ghee in a large nonstick skillet over medium-high. Add potatoes and cook, undisturbed, until a deep golden crust forms on bottom, about 5 minutes. Break up potatoes with a heatproof rubber spatula and continue to cook, turning occasionally with spatula and adding 1–2 Tbsp. clarified butter or ghee if pan becomes dry or potatoes start to stick, until crisped and browned all over, 8–10 minutes. Transfer to paper towels to drain; season with salt.']</t>
         </is>
       </c>
-      <c r="E67" t="inlineStr">
+      <c r="F67" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/57acf1d2f1c801a1038bc928/16:9/w_940,c_limit/ba-best-hash-browns.jpg</t>
         </is>
@@ -2183,15 +2518,20 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
+          <t>Our idea of magic mushrooms is crisp, golden (legal) substances with the power to lend a bass note of flavor to grain salads, turn a piece of ricotta toast into a meal, or stand alone as a savory side. Learn how to make this recipe and more in our online cooking class with Sur la Table.</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
           <t>['2 tablespoons olive oil', '12 ounces mushrooms (such as maitake, oyster, and/or king trumpet), cut into large pieces', 'Kosher salt, freshly ground pepper', '4 tablespoons unsalted butter, cut into pieces', '2 sprigs thyme', '2 garlic cloves, crushed']</t>
         </is>
       </c>
-      <c r="D68" t="inlineStr">
+      <c r="E68" t="inlineStr">
         <is>
           <t>['Heat oil in a large skillet over medium-high until just beginning to smoke. Arrange mushrooms in skillet in a single layer and cook, undisturbed, until bottom side is golden brown, about 3 minutes. Season with salt and pepper, toss mushrooms, and continue to cook, tossing often and reducing heat as needed to avoid scorching, until golden brown all over, about 5 minutes more.', 'Reduce heat to medium and add butter, thyme sprigs, and garlic to skillet. Tip skillet toward you so butter pools at bottom edge. Spoon foaming butter over mushrooms until butter smells nutty, about 4 minutes. Remove mushrooms from skillet with a slotted spoon.']</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr">
+      <c r="F68" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/57acdbf41b33404414975275/16:9/w_940,c_limit/seared-mushrooms-with-garlic-and-thyme.jpg</t>
         </is>
@@ -2210,15 +2550,20 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
+          <t>Halloumi has a firm, squeaky texture and high melting point and tastes like a mild feta cheese. If you can’t find it, look for queso blanco, “grilling cheese,” or bread cheese instead.</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
           <t>['1 tablespoon olive oil, plus more', '1 8.8-ounce package Halloumi cheese, cut into 1-inch pieces', '1 teaspoon fresh thyme leaves', '½ teaspoon crushed red pepper flakes', '1 cup oil-cured black olives, pitted']</t>
         </is>
       </c>
-      <c r="D69" t="inlineStr">
+      <c r="E69" t="inlineStr">
         <is>
           <t>['Heat a medium skillet, preferably cast iron or nonstick, over medium. Add 1 Tbsp. oil and swirl to coat pan. Add Halloumi and cook undisturbed until cheese is deep golden brown, about 2 minutes. Using a thin flexible spatula, release cheese from skillet and toss. Cook, tossing occasionally, until a few more sides are golden brown, about 5 minutes (don’t worry about getting all sides browned).', 'Remove skillet from heat and toss in thyme and red pepper flakes. Divide Halloumi mixture and olives among small plates and drizzle with more oil.']</t>
         </is>
       </c>
-      <c r="E69" t="inlineStr">
+      <c r="F69" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/57acd42c1b33404414975217/16:9/w_940,c_limit/halloumi-with-cured-olives-and-thyme.jpg</t>
         </is>
@@ -2237,15 +2582,20 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
+          <t>Make sure the leftover greens, especially if you’re using kale, are totally softened—you should be able to cut through them easily.</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
           <t>['2 tablespoons unsalted butter, divided', '4 large eggs, beaten to blend, divided', 'Kosher salt, freshly ground pepper', '⅓ cup Muenster cheese, shredded, divided', '4 ounces loose chicken-apple sausage, cooked, divided', '⅓ cup sautéed greens (such as spinach, kale, or Swiss chard), divided']</t>
         </is>
       </c>
-      <c r="D70" t="inlineStr">
+      <c r="E70" t="inlineStr">
         <is>
           <t>['Melt 1 Tbsp. butter in an 8" nonstick skillet over medium heat. Season eggs with salt and pepper.', 'Add half of eggs to skillet. Cook eggs, stirring gently with a heatproof spatula, until eggs are lightly scrambled and almost cooked through, about 3 minutes. Spread eggs evenly to cover bottom of skillet.', 'Top eggs with half of Muenster, sausage, and greens. Using spatula, fold over one-third of omelet. Roll omelet onto itself, then slide onto a plate. Repeat with remaining ingredients to make a second omelet.']</t>
         </is>
       </c>
-      <c r="E70" t="inlineStr">
+      <c r="F70" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/57acdd4953e63daf11a4dadd/16:9/w_940,c_limit/BACK-TO-SCHOOL-OMELETTE-1-of-1.jpg</t>
         </is>
@@ -2264,15 +2614,20 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
+          <t>The strawberry syrup is perfect for topping ice cream and yogurt, or mix about 3 Tbsp. into room-temperature butter for spreading onto biscuits, pancakes, and French toast.</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
           <t>['1 pound strawberries, hulled, quartered', '¾ cup sugar', '½ vanilla bean, split lengthwise, or 1½ teaspoons vanilla extract', 'Milk (for serving)']</t>
         </is>
       </c>
-      <c r="D71" t="inlineStr">
+      <c r="E71" t="inlineStr">
         <is>
           <t>['Bring strawberries, sugar, and ¼ cup water to a boil over medium heat, then reduce heat and simmer, skimming occasionally, until strawberries are soft and fragrant, about 10 minutes. Remove from heat and add vanilla bean. Let cool completely, at least 1 hour.', 'Strain strawberry mixture through a fine-mesh sieve into a small bowl, pressing strawberries to extract as much juice as possible; discard solids, then chill syrup at least 1 hour. To serve, stir ¼ cup syrup into 1 cup milk.', 'Do Ahead: Strawberry syrup can be made 1 week ahead. Store in an airtight container and chill.']</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr">
+      <c r="F71" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/57acdd9553e63daf11a4dade/16:9/w_940,c_limit/BACK-TO-SCHOOL-4-of-1.jpg</t>
         </is>
@@ -2291,15 +2646,20 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
+          <t>Try this in a frittata, folded into a grain salad, or in a hash with bacon. Learn how to make this recipe and more in our online cooking class with Sur la Table.</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
           <t>['2 small heads of broccoli, cut into florets with some stalk attached, or 1 medium acorn squash, seeds removed, cut into ½-inch slices', '2 tablespoons virgin coconut oil, warmed to liquefy if needed', 'Kosher salt, freshly ground pepper', '2 tablespoons nutritional yeast']</t>
         </is>
       </c>
-      <c r="D72" t="inlineStr">
+      <c r="E72" t="inlineStr">
         <is>
           <t>['Preheat oven to 425°. Toss vegetables with oil on a rimmed baking sheet to coat; season with salt and pepper. Roast until deep golden brown and tender, 20–25 minutes. Let cool slightly, then toss with nutritional yeast.', 'Do Ahead: Veggies can be made 5 days ahead. Cover and chill.']</t>
         </is>
       </c>
-      <c r="E72" t="inlineStr">
+      <c r="F72" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/57accee9f1c801a1038bc7a4/16:9/w_940,c_limit/roasted-veg-with-nutritional-yeast.jpg</t>
         </is>
@@ -2318,15 +2678,20 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
+          <t>Gjelina chef Travis Lett prefers Hachiya persimmons for this fabulously simple dessert (they’re the ones with the pointy shape). But don’t use them until they’re super soft and completely ripe; they taste unpleasantly tannic otherwise.</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
           <t>['2 cups plain Greek yogurt', '4 ripe Hachiya persimmons, each cut into 6 wedges', '¼ cup finely chopped unsalted, shelled raw pistachios', '⅓ cup buckwheat or clover honey', 'Flaky sea salt (such as Maldon)']</t>
         </is>
       </c>
-      <c r="D73" t="inlineStr">
+      <c r="E73" t="inlineStr">
         <is>
           <t>['Divide yogurt among plates or bowls. Top with persimmons and pistachios, drizzle with honey, and sprinkle with salt.']</t>
         </is>
       </c>
-      <c r="E73" t="inlineStr">
+      <c r="F73" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/57add90d1b334044149756c5/16:9/w_940,c_limit/persimmons-with-greek-yogurt-and-pistachios.jpg</t>
         </is>
@@ -2345,15 +2710,20 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
+          <t>Why waste time with a knife? A simple whack to a cucumber yields jagged surfaces eager to soak up this tangy dressing.</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
           <t>['1 pound Persian or English hothouse cucumbers', '1 teaspoon kosher salt, plus more', '3 scallions, sliced', '3 tablespoons unseasoned rice vinegar', '1 teaspoon toasted sesame seeds', 'Chili oil (for serving)']</t>
         </is>
       </c>
-      <c r="D74" t="inlineStr">
+      <c r="E74" t="inlineStr">
         <is>
           <t>['Gently smack cucumbers with a rolling pin or the bottom of a heavy pot until they begin to break apart. Tear into bite-size pieces. Transfer to a colander; toss with 1 tsp. salt. Let sit 10 minutes to drain excess liquid.', 'Transfer cucumbers to a medium bowl and toss with scallions, rice vinegar, and sesame seeds. Taste and adjust seasoning with salt. Drizzle with chili oil.']</t>
         </is>
       </c>
-      <c r="E74" t="inlineStr">
+      <c r="F74" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/57acea9253e63daf11a4db79/16:9/w_940,c_limit/cucumbers-with-scallions-and-chili-oil.jpg</t>
         </is>
@@ -2372,15 +2742,20 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
+          <t>Along with salt and pepper, lemons are all you need to season everything from simple pastas to poached fish.</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
           <t>['Olive oil (for poaching; about 3½ cups)', '4 6–7-ounce skin-on trout fillets, pin bones removed, room temperature', 'Lemon wedges (for serving)', 'Flaky sea salt']</t>
         </is>
       </c>
-      <c r="D75" t="inlineStr">
+      <c r="E75" t="inlineStr">
         <is>
           <t>['Pour oil into a large skillet to come ¾" up sides and heat over medium until an instant-read thermometer registers 160°. Carefully slip trout into oil, skin side down, and cook, adjusting heat to maintain temperature at 160°, until just opaque, about 3 minutes.', 'Using a fish spatula, transfer trout to a baking sheet, placing skin side up. Blot away excess oil with paper towels. Squeeze lemon juice over both sides of each fillet, then season with salt. Serve with additional lemon wedges for squeezing over.']</t>
         </is>
       </c>
-      <c r="E75" t="inlineStr">
+      <c r="F75" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/57accf841b334044149751ec/16:9/w_940,c_limit/olive-oil-poached-trout.jpg</t>
         </is>
@@ -2399,15 +2774,20 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
+          <t>Some coconut waters have a blush to them, so look for white or clear ones for making this punch recipe. And yes, you can serve this in a punch bowl if you don't have any coconut shells lying around!</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
           <t>['1 750-ml bottle dry gin (preferably J. Rieger &amp; Co.)', '6 cups coconut water', '¾ cup fresh lime juice', '¾ cup (or more) sugar', '¼ cup dry curaçao liqueur (preferably Pierre Ferrand)', '8–12 coconut shells (optional)', 'Mint sprigs and lime wedges (for serving)']</t>
         </is>
       </c>
-      <c r="D76" t="inlineStr">
+      <c r="E76" t="inlineStr">
         <is>
           <t>['Whisk gin, coconut water, lime juice, sugar, and curaçao in a large bowl until sugar is dissolved. Taste and add more sugar, if desired. Chill until cold, at least 1 hour and up to 4 hours.', 'If serving punch in coconut shells, use a hacksaw or cleaver to cut 2" off the tops: Working one at a time, saw part of the way through as you rotate the shell, or use the back of the cleaver to whack as you rotate. Keep working your way around the shell until it cracks open. You won’t get a perfectly smooth cut and that’s okay.', 'Ladle punch into ice-filled coconut shells or rocks glasses and garnish each with a mint sprig and a lime wedge.']</t>
         </is>
       </c>
-      <c r="E76" t="inlineStr">
+      <c r="F76" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/596a5b4d6c75df51bc0b91f7/16:9/w_940,c_limit/barbados-gin-punch.jpg</t>
         </is>
@@ -2426,15 +2806,20 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
+          <t>This two-technique solution—baking first, then finishing under the broiler—yields perfectly browned fish and tender vegetables.</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
           <t>['6 tablespoons olive oil', '2 tablespoons harissa paste', '6 spring onions, halved lengthwise, or 8 scallions (left whole)', '1 pound new potatoes or small potatoes, scrubbed, thinly sliced', 'Kosher salt and freshly ground black pepper', '1½ pounds skin-on snapper fillets (3–4)', 'Lemon wedges (for serving)']</t>
         </is>
       </c>
-      <c r="D77" t="inlineStr">
+      <c r="E77" t="inlineStr">
         <is>
           <t>['Place an oven rack in upper third of oven; preheat to 425°. Combine oil and harissa in a small bowl; adjust flavor with more harissa if needed (spiciness and flavor vary from brand to brand).', 'Toss onions and potatoes with half of harissa mixture in a large baking dish; season with salt and pepper, then add ¼ cup water. Roast, tossing once, until potatoes are fork-tender, 20–25 minutes.', 'Meanwhile, score skin side of fillets about ¼" deep; season with salt and pepper. Rub remaining harissa mixture all over fish, getting into the score marks.', 'Remove onions and potatoes from oven and heat broiler. Place fish skin side up on top of vegetables and broil until onions and potatoes are tender and fish is cooked through and starting to brown on top, 8–10 minutes.', 'Serve fish and vegetables with lemon wedges for squeezing over.']</t>
         </is>
       </c>
-      <c r="E77" t="inlineStr">
+      <c r="F77" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/57acec6c53e63daf11a4db94/16:9/w_940,c_limit/baked-snapper-with-harissa-new-potatoes-and-spring-onions.jpg</t>
         </is>
@@ -2453,15 +2838,20 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
+          <t>Choose a mild and creamy Gorgonzola for this dip.</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
           <t>['4 ounces Gorgonzola Dolce', '4 ounces cream cheese', '¾ cup heavy cream', 'Kosher salt and freshly ground black pepper', 'Crudités (such as sliced fennel, sliced baby beets, radishes with tops, cucumbers, and small carrots with tops) and toast points (for serving)']</t>
         </is>
       </c>
-      <c r="D78" t="inlineStr">
+      <c r="E78" t="inlineStr">
         <is>
           <t>['Pulse Gorgonzola, cream cheese, and cream in a food processor until smooth; season with salt and pepper. Serve with crudités and toast points alongside.', 'Do Ahead: Dip can be made 5 days ahead. Cover and chill; let sit at room temperature 20 minutes before serving.']</t>
         </is>
       </c>
-      <c r="E78" t="inlineStr">
+      <c r="F78" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/57ace6c353e63daf11a4db50/16:9/w_940,c_limit/whipped-gorgonzola.jpg</t>
         </is>
@@ -2480,15 +2870,20 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
+          <t xml:space="preserve">The initial charring of the cabbage is key: Be brave. If you think you’ve made a terrible mistake and burned dinner, you’re doing something right. </t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
           <t>['2 1-inch pieces dried kombu', '1 tablespoon grapeseed oil', '1 medium pointed cabbage or green cabbage (about 1½ pounds), outer leaves removed', '4 tablespoons (½ stick) unsalted butter', '10 basil leaves', '2 teaspoons apple cider vinegar', 'Kosher salt', 'A spice mill or a mortar and pestle']</t>
         </is>
       </c>
-      <c r="D79" t="inlineStr">
+      <c r="E79" t="inlineStr">
         <is>
           <t>['Grind kombu in a spice mill or with a mortar and pestle to a fine powder. (You should have about ¾ tsp.) Heat oil in a medium heavy skillet (such as carbon steel or cast iron) over medium-high and add half of cabbage, cut side down (reserve remaining half for another use). Cook cabbage, undisturbed, until underside is almost blackened (the edge of the sides will start to brown as well), 10–15 minutes.', "Reduce heat to medium-low, add butter to skillet, and shake pan to help butter get in, around, and under cabbage. As soon as butter is melted and foaming, tilt skillet toward you and spoon browning butter over cabbage, being sure to bathe the area around the core (thick and dense, this part will take the longest to cook), 30 seconds. Stop basting and let cabbage cook, undisturbed, 3 minutes, then baste again, 30 seconds more. Repeat cooking and basting process twice more (butter will continue to get darker as it cooks, and that's okay; add a knob or two more to bring it back from the brink), adding kelp to brown butter just before final basting. At this point, cabbage should be tender (a cake tester or skewer inserted into the core should meet with no resistance) and the outer leaves have pulled away from one another. If cabbage is not done, repeat cooking and basting process once more.", 'Transfer cabbage to a cutting board and cut into two quarters. Pull leaves open slightly and tuck basil here and there between a few leaves. Drizzle with vinegar and season with salt. Let cabbage sit a minute or two for basil to soften before serving.']</t>
         </is>
       </c>
-      <c r="E79" t="inlineStr">
+      <c r="F79" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/57acf29c1b33404414975372/16:9/w_940,c_limit/blackened-cabbage-with-kelp-brown-butter.jpg</t>
         </is>
@@ -2507,15 +2902,20 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
+          <t>Red snapper, salmon, and pompano are also good choices if you can't find branzino or mackerel. Learn more here.</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
           <t>['2 6-ounce fillets branzino or mackerel', '2 tablespoons vegetable oil, divided', 'Kosher salt', 'Mixed Olive Vinaigrette']</t>
         </is>
       </c>
-      <c r="D80" t="inlineStr">
+      <c r="E80" t="inlineStr">
         <is>
           <t>['Place fish on a plate, skin side up, and chill, uncovered for one hour. (This dries out the skin and is a crucial step.)', 'Heat a large stainless-steel skillet over high. Once the skillet is extremely hot, about 2 minutes, add 1 Tbsp. oil and a large pinch of salt. Heat oil until smoking, then remove skillet from heat and wipe out with a clean kitchen towel (this creates a temporary seal on the pan, like a faux nonstick surface).', "Season both sides of fillets with salt. Return skillet to high heat and add remaining 1 Tbsp. oil. Once oil is hot and shimmering, add 1 fillet, lowering it into the pan away from you, skin side down. Press gently with a spatula until fillet no longer wants to curl up and entire skin side is flush with the skillet, ensuring complete and direct contact. Repeat with remaining fillet. Cook fish, pressing periodically with spatula, until fish is nearly cooked through (it should still be opaque and a bit raw at the thickest part of the fillet), about 3 minutes. Gently turn fish (working away from you so the oil doesn't splash on you) and finish cooking off heat, about another minute or so.", 'To serve, spoon a bit of vinaigrette onto plates and place fish on top, skin side up (no point in working so hard to create a beautifully crisp skin only to cover it up with sauce!).']</t>
         </is>
       </c>
-      <c r="E80" t="inlineStr">
+      <c r="F80" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/57acf370f1c801a1038bc943/16:9/w_940,c_limit/crispy-skinned-fish2.jpg</t>
         </is>
@@ -2534,15 +2934,20 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
+          <t>Garlicky, pungent ramps set off pesto pyrotechnics.</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
           <t>['4 ounces ramps, greens separated', 'Kosher salt', '12 ounces spaghetti', '¼ cup walnuts, toasted', '⅓ cup olive oil', '2 tablespoons grated Pecorino, plus more for serving', 'Lemon wedges, for serving']</t>
         </is>
       </c>
-      <c r="D81" t="inlineStr">
+      <c r="E81" t="inlineStr">
         <is>
           <t>['Blanch ramp greens in a large pot of boiling salted water until wilted, about 10 seconds. Using a slotted spoon or spider, transfer greens to a bowl of ice water; drain and squeeze out liquid.', 'Bring same water in pot to a boil again and cook spaghetti, stirring occasionally, until al dente; drain, reserving 1 cup pasta cooking liquid.', 'Meanwhile, coarsely chop ramp bulbs and stalks (save or pickle the rest) and walnuts in a food processor.', 'Add ramp greens, olive oil, and 2 Tbsp. Pecorino; process to a coarse paste. Season with salt.', 'Toss spaghetti and ½ cup cooking liquid with pesto, adding more cooking liquid as needed until pesto coats pasta. Serve topped with more Pecorino and with lemon wedges.']</t>
         </is>
       </c>
-      <c r="E81" t="inlineStr">
+      <c r="F81" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/57acf21153e63daf11a4dbc1/16:9/w_940,c_limit/ramp-pesto-spaghetti.jpg</t>
         </is>
@@ -2561,15 +2966,20 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
+          <t>This is your mainstay recipe for perfect roasted Brussels sprouts. For more variations and veggie inspiration, check out our roasted veggie matrix.</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
           <t>['3 pounds brussels sprouts, trimmed, halved, quartered if large', '5 tablespoons olive oil', '2 teaspoons kosher salt', '½ teaspoon freshly ground black pepper']</t>
         </is>
       </c>
-      <c r="D82" t="inlineStr">
+      <c r="E82" t="inlineStr">
         <is>
           <t>['Preheat oven to 450°. Toss brussels sprouts, oil, salt, and pepper on a rimmed baking sheet. Roast, tossing occasionally, until tender and browned, 35–45 minutes.']</t>
         </is>
       </c>
-      <c r="E82" t="inlineStr">
+      <c r="F82" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/57acd5d953e63daf11a4da7f/16:9/w_940,c_limit/ROAST-VEG-1-of-7.jpg</t>
         </is>
@@ -2588,15 +2998,20 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
+          <t>If you close your eyes, you’ll swear this frozen custard recipe tastes exactly like pink lemonade.</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
           <t>['3 tablespoons dried hibiscus flowers or hibiscus tea', '2½ cups heavy cream', '2 tablespoons finely grated lemon zest', '½ cup plus 2 tablespoons sugar', '¼ teaspoon kosher salt', '6 large egg yolks', '¼ cup fresh lemon juice']</t>
         </is>
       </c>
-      <c r="D83" t="inlineStr">
+      <c r="E83" t="inlineStr">
         <is>
           <t>['Steep hibiscus in ½ cup very hot water in a small bowl for 10 minutes. Strain into another small bowl, pressing on solids to extract all liquid; let cool.', 'Meanwhile, bring cream, lemon zest, and ½ cup sugar to a bare simmer in a medium saucepan. Remove from heat, cover, and let stand 10 minutes.', 'Whisk salt and remaining 2 Tbsp. sugar into egg yolks in a medium bowl to blend. Return cream mixture to a simmer, then slowly pour into egg mixture, whisking constantly until incorporated. Return to saucepan and cook over medium heat, stirring constantly with a wooden spoon and scraping bottom of pan, until thick enough to coat spoon, 5–7 minutes.', 'Strain into a large bowl (preferably metal; custard will cool down more quickly) set over a bowl of ice water. Let cool, stirring occasionally. Stir in lemon juice and hibiscus infusion. Process custard in an ice cream maker according to manufacturer’s instructions. Freeze in an airtight container until firm, at least 4 hours.', 'DO AHEAD: Frozen custard can be made 2 weeks ahead. Keep frozen.']</t>
         </is>
       </c>
-      <c r="E83" t="inlineStr">
+      <c r="F83" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/57acf898f1c801a1038bc97c/16:9/w_940,c_limit/lemon-hibiscus-frozen-custard.jpg</t>
         </is>
@@ -2615,15 +3030,20 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
+          <t>After rigorous scientific testing for this best-ever grilled cheese, we’ve determined that sandwiches sliced in half on a diagonal actually taste better.</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
           <t>['2 slices ½”-thick Pullman or other white bread', '2 tablespoons mayonnaise', '1 tablespoon unsalted butter', '2 ounces thinly sliced American cheese or cheddar (about 4 slices)', 'Freshly ground black pepper', 'Campbell’s Tomato Soup (for serving; optional)']</t>
         </is>
       </c>
-      <c r="D84" t="inlineStr">
+      <c r="E84" t="inlineStr">
         <is>
           <t>['Place bread on a cutting board and spread mayonnaise over top side of each; this is key to a golden, delectable crunch. Heat a small skillet (nonstick, ideally) over medium. Slide in half of butter. When it melts, place 1 slice of bread, mayonnaise side down, in skillet; top with cheese; season with pepper. Top with second slice of bread, mayonnaise side up. When underside is golden brown, about 4 minutes, turn sandwich and add remaining butter to skillet. Press down on sandwich to encourage even browning and to help melt cheese—be gentle, don’t smash it. Cook until second side is golden brown and cheese is melted. Eat immediately, preferably with soup.']</t>
         </is>
       </c>
-      <c r="E84" t="inlineStr">
+      <c r="F84" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/57acf62a53e63daf11a4dbee/16:9/w_940,c_limit/best-ever-grilled-cheese.jpg</t>
         </is>
@@ -2642,15 +3062,20 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
+          <t>If you’ve got a microwave, you can cook the potatoes in less time, but use the oven for the second bake.</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
           <t>['4 large russet potatoes', '2 tablespoons vegetable oil', '½ cup sour cream', '¼ cup unsalted butter', '¼ cup finely chopped fresh chives', '1 tablespoon finely chopped fresh tarragon (optional)', 'Kosher salt and freshly ground black pepper']</t>
         </is>
       </c>
-      <c r="D85" t="inlineStr">
+      <c r="E85" t="inlineStr">
         <is>
           <t>['Place a rack in middle of oven; preheat to 425°. Poke potatoes all over with a fork; rub with oil. Bake directly on oven rack until very soft when squeezed and skins are crisp, 50–60 minutes. Let cool just until you can hold them.', 'Using a serrated knife, slice potatoes in half lengthwise and scoop flesh into a medium bowl. Add sour cream, butter, chives, and tarragon (if desired); season generously with salt and pepper.', 'Divide among 4 potato skin halves, piling gloriously high—don’t pack too tightly. (And what about the leftover skins? We say add butter and salt and snack on them.)', 'Increase oven temperature to 450°. Bake potatoes on a rimmed baking sheet until filling is puffed and browned in spots, 20–25 minutes.']</t>
         </is>
       </c>
-      <c r="E85" t="inlineStr">
+      <c r="F85" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/57acf6e5f1c801a1038bc96e/16:9/w_940,c_limit/twice-baked-potatoes.jpg</t>
         </is>
@@ -2669,15 +3094,20 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
+          <t>After the beet has given up its color for the eggs, it’s a great addition to a salad.</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
           <t>['4 cups distilled white vinegar', '½ cup sugar', '1 tablespoon kosher salt', '1 large red beet, peeled, cut into ¼-inch pieces', '4 hard-boiled eggs, peeled']</t>
         </is>
       </c>
-      <c r="D86" t="inlineStr">
+      <c r="E86" t="inlineStr">
         <is>
           <t>['Bring vinegar, sugar, salt, and 2½ cups water to a boil in a large saucepan, stirring to dissolve sugar and salt. Add beet, reduce heat, and simmer until beet is tender, 25–30 minutes. Let cool, then strain brine into a resealable glass jar. Add eggs to brine; reserve beet for another use. Chill eggs at least 2 hours before serving.', 'Do Ahead: Eggs can be pickled 2 days ahead. Keep chilled.']</t>
         </is>
       </c>
-      <c r="E86" t="inlineStr">
+      <c r="F86" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/57acdfc153e63daf11a4dafa/16:9/w_940,c_limit/beet-pickled-eggs1.jpg</t>
         </is>
@@ -2696,15 +3126,20 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
+          <t>At Pirelli's restaurant in Rome, chef Barbara Lynch ate what was, for her, the perfect carbonara: The sauce was bright yellow from fresh eggs, and each rigatoni hid cubes of fatty guanciale. In Boston, where Lynch has five restaurants, she set out to master the dish. Her yolk-heavy recipe is beyond creamy—without cream!—with a heady mix of peppercorns (you can substitute black pepper for all and it's still great). It's unlike any clumpy carbonaras you've had. The tricks? She omits most of the egg whites; their water thins the sauce. Too much cheese overthickens it, so she gradually adds Pecorino while tossing the pasta until she hits the right consistency (the sauce should be loose enough to drag the pasta through). Lynch was right: It's a pasta worth mastering. This is part of BA's Best, a collection of our essential recipes.</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
           <t>['¼ pound guanciale (salt-cured pork jowl) or pancetta, cut into ⅓-inch cubes', '7 large egg yolks', '1 large egg', '1 pound rigatoni', 'Kosher salt', '½ cup finely grated Pecorino or Parmesan, plus more for garnish', '2 teaspoons freshly ground black pepper (or ¾ teaspoon freshly ground green peppercorns plus ¾ teaspoon freshly ground pink peppercorns plus ½ teaspoon freshly ground white peppercorns), plus more']</t>
         </is>
       </c>
-      <c r="D87" t="inlineStr">
+      <c r="E87" t="inlineStr">
         <is>
           <t>['Cook guanciale in a large skillet over medium-low heat, stirring frequently, until fat renders but guanciale is not browned, about 5 minutes. Pour into a fine-mesh sieve set over a small bowl; reserve drippings. Transfer guanciale to a large bowl and let cool slightly. Add egg yolks and egg to bowl; whisk to blend.', 'Meanwhile, cook pasta in a large pot of boiling salted water, stirring occasionally, until al dente. Drain, reserving ½ cup pasta cooking liquid.', 'Immediately add rigatoni, 2 Tbsp. pasta cooking liquid, and 1 tsp. guanciale drippings to egg mixture; toss to coat. Working in 3 batches, gradually add ½ cup Pecorino, stirring and tossing to melt between batches. Add 2 tsp. black pepper; toss until sauce thickens, adding more pasta water by tablespoonfuls if needed. Season with salt and pepper.', 'Divide among bowls. Garnish with Pecorino.']</t>
         </is>
       </c>
-      <c r="E87" t="inlineStr">
+      <c r="F87" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/57af6fa753e63daf11a4e5a0/16:9/w_940,c_limit/11112015-WEB-SHOOT-010.jpg</t>
         </is>
@@ -2723,15 +3158,20 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
+          <t>Crispy, salty, creamy, and full of protein (really!), these chickpeas should be a staple in your kitchen.</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
           <t>['2 15.5-ounce cans chickpeas, rinsed, patted dry', '4 garlic cloves, crushed', '⅓ cup olive oil', 'Kosher salt, freshly ground pepper', '2½ cups chopped mixed tender herbs (such as parsley, cilantro, chives, and/or basil)']</t>
         </is>
       </c>
-      <c r="D88" t="inlineStr">
+      <c r="E88" t="inlineStr">
         <is>
           <t>['Place chickpeas in a large skillet or Dutch oven and add garlic and oil; season with salt and pepper. Cook over medium heat, stirring occasionally, until chickpeas are crisped and some have split open (these will be the most delicious ones), 10–15 minutes. Remove from heat; stir in herbs.']</t>
         </is>
       </c>
-      <c r="E88" t="inlineStr">
+      <c r="F88" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/57acd1d0f1c801a1038bc7ce/16:9/w_940,c_limit/herbed-chickpeas.jpg</t>
         </is>
@@ -2750,15 +3190,20 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
+          <t>Call us crazy, but we think these three-ingredient charred ribs are just as delicious (if not more so!) than the low-and-slow, fall-off-the-bone-tender kind. They develop a crispy crust as they cook for just 15 minutes on each side, and despite the ridiculously short ingredient list, they’re still plenty flavorful and juicy due to the high fat content in the ribs.</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
           <t>['3 lb. baby back pork ribs (1–2 racks)', 'Kosher salt, freshly ground pepper']</t>
         </is>
       </c>
-      <c r="D89" t="inlineStr">
+      <c r="E89" t="inlineStr">
         <is>
           <t>['Let ribs sit at room temperature 30 minutes. Cut pork between rib bones into 2- or 3-rib sections. Pat dry with paper towels. Season both sides generously with salt and pepper (about 1½ tsp. Diamond Crystal or 1 tsp. Morton kosher salt per 1 lb. ribs; check the butcher’s label on your package for the weight).', 'Prepare a gas or charcoal grill for medium heat. (To check that your grill is at medium heat, hold your hand about 5" above the grate; you should be able to stay there 7–8 seconds before it’s too hot and you have to move your hand away.)', 'Grill ribs bone side down until deep golden brown, about 15 minutes. Turn ribs and continue to grill until golden brown and crisp, about 15 minutes more.', 'Cut between bones into single ribs and transfer to a platter.Photo by Chelsie Craig, Food Styling by Pearl Jones']</t>
         </is>
       </c>
-      <c r="E89" t="inlineStr">
+      <c r="F89" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/5d6400a45ec6b10008568f8b/16:9/w_940,c_limit/BA-0819-Ribs-lede.jpg</t>
         </is>
@@ -2777,15 +3222,20 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
+          <t>You’re not going to get this right the first time. After five, maybe six attempts, you’ll start to feel like a pro. This is part of BA's Best, a collection of our essential recipes. Check out the step-by-step here and watch the video here.</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
           <t>['2 large eggs', '2 tablespoons unsalted European-style butter (such as Plugra), room temperature, divided, plus more for serving', 'Fleur de sel or other coarse sea salt', 'Freshly ground white pepper', '1 ounce Boursin Pepper Cheese', '1 tablespoon finely chopped chives']</t>
         </is>
       </c>
-      <c r="D90" t="inlineStr">
+      <c r="E90" t="inlineStr">
         <is>
           <t>['Whisk eggs in a medium bowl until very, very well combined (there should be no strands of egg white remaining, but be careful not to incorporate too much air). To make sure eggs are really smooth, strain through a fine-mesh sieve into a small bowl.', 'Heat 1 Tbsp. butter in an 8" nonstick skillet over medium heat. Once the butter just begins to foam (don\'t let it sizzle), add eggs and season with fleur de sel and pepper. Using a rubber spatula, stir eggs very quickly and constantly in a figure-eight pattern while simultaneously moving the skillet around in a circular motion. Scrape down the sides of the skillet as you go to avoid dry bits in your omelet.', 'As soon as eggs begin to coagulate, which will take about 2 minutes, shake skillet to settle any uncooked egg. Keep stirring and moving pan in a circular motion until eggs are nearly cooked through on the bottom but still runny on top (or baveuse, as the French say), about 1 minute. Lift an edge of the omelet to check that it is holding together; the underside of the omelet should have taken on no color. Remove pan from heat and let sit 1 minute to help omelet release from skillet and maintain its smooth texture.', "Spoon dollops of cheese across the center of the omelet, working perpendicular to the skillet's handle, setting you up to hold the handle with your left hand and flip the omelet onto your plate when the time comes.", 'Starting at the edge closest to the handle, immediately roll up omelet in 1½" intervals, using spatula, until halfway through. Add another 1 Tbsp. butter, then continue rolling up omelet and turn out onto a plate, seam side down.', 'Rub a little butter on top of omelet (to make it shiny) and sprinkle with fleur de sel and chives.']</t>
         </is>
       </c>
-      <c r="E90" t="inlineStr">
+      <c r="F90" t="inlineStr">
         <is>
           <t>https://assets.bonappetit.com/photos/57acf3e21b33404414975388/16:9/w_940,c_limit/ludos-omelet1.jpg</t>
         </is>

</xml_diff>